<commit_message>
fix random generator bug
</commit_message>
<xml_diff>
--- a/project4/Workbook1.xlsx
+++ b/project4/Workbook1.xlsx
@@ -181,220 +181,220 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="72"/>
                 <c:pt idx="0">
-                  <c:v>32.189884</c:v>
+                  <c:v>20.885609</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>27.234589</c:v>
+                  <c:v>44.223167</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>54.019173</c:v>
+                  <c:v>44.351357</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>58.216587</c:v>
+                  <c:v>56.799408</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>70.50108299999999</c:v>
+                  <c:v>59.47784</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>79.072639</c:v>
+                  <c:v>78.363449</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>61.173187</c:v>
+                  <c:v>66.63443</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>72.406998</c:v>
+                  <c:v>71.83225299999999</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>56.750648</c:v>
+                  <c:v>55.859356</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>36.69286</c:v>
+                  <c:v>52.973492</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>36.807289</c:v>
+                  <c:v>36.07563</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>25.537155</c:v>
+                  <c:v>22.409046</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>36.750443</c:v>
+                  <c:v>28.810452</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>34.712334</c:v>
+                  <c:v>35.202602</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>42.515759</c:v>
+                  <c:v>36.033852</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>58.0466</c:v>
+                  <c:v>57.877426</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>70.682129</c:v>
+                  <c:v>73.272003</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>62.826061</c:v>
+                  <c:v>61.035522</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>64.54287</c:v>
+                  <c:v>76.67607099999999</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>68.095367</c:v>
+                  <c:v>56.042229</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>54.340782</c:v>
+                  <c:v>56.298615</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>41.606369</c:v>
+                  <c:v>52.726635</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>32.09864</c:v>
+                  <c:v>39.937725</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>28.382578</c:v>
+                  <c:v>29.505066</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>39.996582</c:v>
+                  <c:v>40.043243</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>27.974194</c:v>
+                  <c:v>44.441383</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>53.898346</c:v>
+                  <c:v>37.164772</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>62.485992</c:v>
+                  <c:v>53.447514</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>64.31353799999999</c:v>
+                  <c:v>56.336689</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>71.178352</c:v>
+                  <c:v>61.941589</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>64.037422</c:v>
+                  <c:v>62.202953</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>56.947269</c:v>
+                  <c:v>65.092361</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>59.490402</c:v>
+                  <c:v>54.192947</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>43.007149</c:v>
+                  <c:v>39.65662</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>37.618587</c:v>
+                  <c:v>33.540306</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>25.979164</c:v>
+                  <c:v>40.206387</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>29.115444</c:v>
+                  <c:v>25.644943</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>39.134174</c:v>
+                  <c:v>32.132748</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>47.337044</c:v>
+                  <c:v>44.887669</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>48.110329</c:v>
+                  <c:v>52.063442</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>72.05204000000001</c:v>
+                  <c:v>69.595291</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>64.31809199999999</c:v>
+                  <c:v>77.277084</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>60.346741</c:v>
+                  <c:v>79.27814499999999</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>57.605164</c:v>
+                  <c:v>69.433426</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>61.868671</c:v>
+                  <c:v>56.14666</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>46.711617</c:v>
+                  <c:v>40.579189</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>28.176994</c:v>
+                  <c:v>39.490269</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>20.754875</c:v>
+                  <c:v>36.393768</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>29.549263</c:v>
+                  <c:v>40.176533</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>31.191721</c:v>
+                  <c:v>38.817863</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>41.455032</c:v>
+                  <c:v>36.494812</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>63.766754</c:v>
+                  <c:v>49.995823</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>65.617203</c:v>
+                  <c:v>72.962654</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>72.98822</c:v>
+                  <c:v>71.332481</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>78.380379</c:v>
+                  <c:v>77.568062</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>70.750153</c:v>
+                  <c:v>62.141407</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>47.333176</c:v>
+                  <c:v>60.944805</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>47.341106</c:v>
+                  <c:v>53.533302</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>39.534386</c:v>
+                  <c:v>36.840324</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>21.616539</c:v>
+                  <c:v>38.933479</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>36.482208</c:v>
+                  <c:v>25.768913</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>37.381447</c:v>
+                  <c:v>42.174145</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>49.165344</c:v>
+                  <c:v>50.653114</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>55.318928</c:v>
+                  <c:v>59.465424</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>72.25932299999999</c:v>
+                  <c:v>57.734196</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>66.098129</c:v>
+                  <c:v>77.249756</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>64.745018</c:v>
+                  <c:v>75.87756299999999</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>71.06250799999999</c:v>
+                  <c:v>58.825798</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>45.30983</c:v>
+                  <c:v>54.012955</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>46.398956</c:v>
+                  <c:v>44.467819</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>30.59861</c:v>
+                  <c:v>28.922798</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>21.391582</c:v>
+                  <c:v>29.444271</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -435,220 +435,220 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="72"/>
                 <c:pt idx="0">
-                  <c:v>5.89108</c:v>
+                  <c:v>7.69221</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>11.964766</c:v>
+                  <c:v>9.369195</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>13.729722</c:v>
+                  <c:v>12.331646</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.146072</c:v>
+                  <c:v>11.443724</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>9.205545</c:v>
+                  <c:v>11.681658</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.073514</c:v>
+                  <c:v>7.205046</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>4.74992</c:v>
+                  <c:v>6.164572</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.276696</c:v>
+                  <c:v>3.310365</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.468544</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>1.1484</c:v>
+                  <c:v>1.747986</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>4.304959</c:v>
+                  <c:v>5.477024</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>7.753675</c:v>
+                  <c:v>6.266221</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>11.657179</c:v>
+                  <c:v>11.650181</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>10.162119</c:v>
+                  <c:v>9.882346</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>11.768836</c:v>
+                  <c:v>11.109354</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>9.792253</c:v>
+                  <c:v>11.389172</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>7.831821</c:v>
+                  <c:v>9.115376</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>3.597692</c:v>
+                  <c:v>4.161739</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.16198</c:v>
+                  <c:v>2.749495</c:v>
                 </c:pt>
                 <c:pt idx="20">
+                  <c:v>0.502954</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>1.410454</c:v>
+                </c:pt>
+                <c:pt idx="22">
                   <c:v>0.0</c:v>
                 </c:pt>
-                <c:pt idx="21">
-                  <c:v>1.74689</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>1.504366</c:v>
-                </c:pt>
                 <c:pt idx="23">
-                  <c:v>4.903003</c:v>
+                  <c:v>6.030779</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>7.327188</c:v>
+                  <c:v>8.183876</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>10.088284</c:v>
+                  <c:v>10.889705</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>11.598509</c:v>
+                  <c:v>11.37207</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>10.287411</c:v>
+                  <c:v>12.344517</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>10.36696</c:v>
+                  <c:v>8.98711</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>7.203724</c:v>
+                  <c:v>6.735762</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>4.600742999999999</c:v>
+                  <c:v>6.212763</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.885622</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>1.349844</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.241978</c:v>
+                  <c:v>3.511035</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>6.079806</c:v>
+                  <c:v>5.470838</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>7.482304</c:v>
+                  <c:v>5.740437</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>11.21571</c:v>
+                  <c:v>8.620131000000001</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>12.46418</c:v>
+                  <c:v>11.138714</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>11.959955</c:v>
+                  <c:v>11.950139</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>10.647421</c:v>
+                  <c:v>8.527266</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>7.148934</c:v>
+                  <c:v>7.490772</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>2.741265</c:v>
+                  <c:v>2.76066</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>0.376613</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.0</c:v>
+                  <c:v>1.741386</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.0</c:v>
+                  <c:v>0.953315</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>3.309978</c:v>
+                  <c:v>3.750722</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>5.130077</c:v>
+                  <c:v>5.700414</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>5.709272</c:v>
+                  <c:v>8.208863</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>9.517982</c:v>
+                  <c:v>12.039536</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>12.61899</c:v>
+                  <c:v>11.336789</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>11.431451</c:v>
+                  <c:v>9.816985</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>8.536063</c:v>
+                  <c:v>11.537493</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>6.887579</c:v>
+                  <c:v>9.291742</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>4.977608</c:v>
+                  <c:v>2.453982</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>1.985402</c:v>
+                  <c:v>0.534539</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.011218</c:v>
+                  <c:v>2.132727</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.0</c:v>
+                  <c:v>0.94615</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.0</c:v>
+                  <c:v>0.155928</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>5.543182</c:v>
+                  <c:v>2.707731</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>6.094018</c:v>
+                  <c:v>6.428429</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>11.619752</c:v>
+                  <c:v>9.799537</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>10.157206</c:v>
+                  <c:v>11.14286</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>10.866258</c:v>
+                  <c:v>12.895859</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>11.322287</c:v>
+                  <c:v>10.564777</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>6.571682</c:v>
+                  <c:v>7.641038</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>3.046112</c:v>
+                  <c:v>4.00063</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>0.0</c:v>
+                  <c:v>3.476727</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.0</c:v>
+                  <c:v>1.473742</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.0</c:v>
+                  <c:v>0.156983</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>3.373554</c:v>
+                  <c:v>2.301359</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>5.384652</c:v>
+                  <c:v>5.695426</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -689,25 +689,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="72"/>
                 <c:pt idx="0">
-                  <c:v>2.67161</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>2.380126</c:v>
+                  <c:v>4.866386</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2.002618</c:v>
+                  <c:v>9.583219</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>1.213146</c:v>
+                  <c:v>8.730567000000001</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.302151</c:v>
+                  <c:v>7.380033</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.0</c:v>
+                  <c:v>5.284027</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.0</c:v>
+                  <c:v>2.506233</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.0</c:v>
@@ -716,193 +716,193 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>2.516614</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>5.363503</c:v>
+                  <c:v>2.623839</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>5.844583</c:v>
+                  <c:v>2.348683</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12.386138</c:v>
+                  <c:v>3.886354</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>17.87088</c:v>
+                  <c:v>9.720802000000001</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>24.526276</c:v>
+                  <c:v>16.252264</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>23.452688</c:v>
+                  <c:v>15.89499</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>21.623423</c:v>
+                  <c:v>14.613105</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>19.317709</c:v>
+                  <c:v>12.497744</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>16.099026</c:v>
+                  <c:v>9.530231000000001</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>12.229885</c:v>
+                  <c:v>6.483449</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>8.945304</c:v>
+                  <c:v>3.96916</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>9.922867</c:v>
+                  <c:v>2.527987</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>9.700200000000001</c:v>
+                  <c:v>4.076027</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>9.223026000000001</c:v>
+                  <c:v>5.418653</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>14.719226</c:v>
+                  <c:v>12.405503</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>14.752654</c:v>
+                  <c:v>18.171339</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>13.878945</c:v>
+                  <c:v>24.313232</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>11.80127</c:v>
+                  <c:v>24.033907</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>9.4481</c:v>
+                  <c:v>22.666494</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>6.563159</c:v>
+                  <c:v>20.277622</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3.522316</c:v>
+                  <c:v>17.270281</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.834119</c:v>
+                  <c:v>13.439188</c:v>
                 </c:pt>
                 <c:pt idx="32">
+                  <c:v>10.354922</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>10.220276</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>11.253133</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>15.648157</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>14.396024</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>16.372667</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>20.289347</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>19.656628</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>17.050001</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>13.797719</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>10.162209</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>6.03327</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>2.880991</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>3.95347</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>7.740509999999999</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>12.359107</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>18.900854</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>25.018208</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>30.164852</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>31.024921</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>28.664234</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>25.845161</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>22.072592</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>17.580208</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>13.848255</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>11.155128</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>11.095786</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>13.261982</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>11.838996</c:v>
+                </c:pt>
+                <c:pt idx="61">
+                  <c:v>17.116369</c:v>
+                </c:pt>
+                <c:pt idx="62">
+                  <c:v>17.351397</c:v>
+                </c:pt>
+                <c:pt idx="63">
+                  <c:v>15.098578</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>12.762147</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>9.877728</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>6.0574</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>2.39652</c:v>
+                </c:pt>
+                <c:pt idx="68">
                   <c:v>0.0</c:v>
                 </c:pt>
-                <c:pt idx="33">
-                  <c:v>1.054126</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>2.710956</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>2.898759</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>4.591688</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>11.965224</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>15.907825</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>18.960873</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>17.477585</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>15.330606</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>12.61771</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>9.572415</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>5.98238</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>5.197848</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>4.654184</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>3.387463</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>4.467582</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>7.241262</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>13.801208</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>12.953818</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>11.542775</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>9.349951000000001</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>6.187811</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>2.926322</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>1.886142</c:v>
-                </c:pt>
-                <c:pt idx="57">
-                  <c:v>1.912942</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>3.925192</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>3.523855</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>9.090462</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>15.916678</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>18.615944</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>18.146921</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>16.353876</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>13.757814</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>10.427359</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>6.361273</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>5.461774</c:v>
-                </c:pt>
                 <c:pt idx="69">
-                  <c:v>5.020255</c:v>
+                  <c:v>0.385997</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>5.530427</c:v>
+                  <c:v>0.368448</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>4.459023</c:v>
+                  <c:v>1.427377</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -946,217 +946,217 @@
                   <c:v>36.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>26.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>28.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
                   <c:v>27.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>21.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="6">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16.0</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>11.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>9.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>23.0</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>18.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>15.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>9.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>6.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>6.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>8.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>17.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>27.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>34.0</c:v>
-                </c:pt>
-                <c:pt idx="16">
+                <c:pt idx="24">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="25">
+                  <c:v>22.0</c:v>
+                </c:pt>
+                <c:pt idx="26">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="27">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="28">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="29">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="31">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="33">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="34">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>42.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>46.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
                   <c:v>39.0</c:v>
                 </c:pt>
-                <c:pt idx="17">
-                  <c:v>43.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
+                <c:pt idx="45">
+                  <c:v>30.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>24.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>41.0</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>48.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>51.0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>52.0</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>53.0</c:v>
+                </c:pt>
+                <c:pt idx="57">
+                  <c:v>52.0</c:v>
+                </c:pt>
+                <c:pt idx="58">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="59">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="60">
+                  <c:v>47.0</c:v>
+                </c:pt>
+                <c:pt idx="61">
                   <c:v>46.0</c:v>
                 </c:pt>
-                <c:pt idx="19">
+                <c:pt idx="62">
                   <c:v>48.0</c:v>
                 </c:pt>
-                <c:pt idx="20">
-                  <c:v>47.0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>43.0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>41.0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>39.0</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>37.0</c:v>
-                </c:pt>
-                <c:pt idx="25">
-                  <c:v>40.0</c:v>
-                </c:pt>
-                <c:pt idx="26">
-                  <c:v>42.0</c:v>
-                </c:pt>
-                <c:pt idx="27">
-                  <c:v>44.0</c:v>
-                </c:pt>
-                <c:pt idx="28">
-                  <c:v>44.0</c:v>
-                </c:pt>
-                <c:pt idx="29">
-                  <c:v>41.0</c:v>
-                </c:pt>
-                <c:pt idx="30">
-                  <c:v>35.0</c:v>
-                </c:pt>
-                <c:pt idx="31">
-                  <c:v>27.0</c:v>
-                </c:pt>
-                <c:pt idx="32">
+                <c:pt idx="63">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>50.0</c:v>
+                </c:pt>
+                <c:pt idx="65">
+                  <c:v>49.0</c:v>
+                </c:pt>
+                <c:pt idx="66">
+                  <c:v>45.0</c:v>
+                </c:pt>
+                <c:pt idx="67">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="68">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="69">
                   <c:v>24.0</c:v>
                 </c:pt>
-                <c:pt idx="33">
-                  <c:v>21.0</c:v>
-                </c:pt>
-                <c:pt idx="34">
-                  <c:v>15.0</c:v>
-                </c:pt>
-                <c:pt idx="35">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="36">
-                  <c:v>9.0</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>9.0</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>18.0</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>27.0</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>34.0</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>39.0</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>42.0</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>42.0</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>40.0</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>34.0</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>28.0</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>23.0</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>18.0</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>15.0</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>17.0</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>25.0</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>30.0</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>33.0</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>33.0</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>29.0</c:v>
-                </c:pt>
-                <c:pt idx="56">
+                <c:pt idx="70">
                   <c:v>22.0</c:v>
                 </c:pt>
-                <c:pt idx="57">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="58">
-                  <c:v>12.0</c:v>
-                </c:pt>
-                <c:pt idx="59">
-                  <c:v>10.0</c:v>
-                </c:pt>
-                <c:pt idx="60">
-                  <c:v>9.0</c:v>
-                </c:pt>
-                <c:pt idx="61">
-                  <c:v>15.0</c:v>
-                </c:pt>
-                <c:pt idx="62">
-                  <c:v>24.0</c:v>
-                </c:pt>
-                <c:pt idx="63">
-                  <c:v>32.0</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>38.0</c:v>
-                </c:pt>
-                <c:pt idx="65">
-                  <c:v>42.0</c:v>
-                </c:pt>
-                <c:pt idx="66">
-                  <c:v>43.0</c:v>
-                </c:pt>
-                <c:pt idx="67">
-                  <c:v>42.0</c:v>
-                </c:pt>
-                <c:pt idx="68">
-                  <c:v>36.0</c:v>
-                </c:pt>
-                <c:pt idx="69">
-                  <c:v>30.0</c:v>
-                </c:pt>
-                <c:pt idx="70">
-                  <c:v>25.0</c:v>
-                </c:pt>
                 <c:pt idx="71">
-                  <c:v>22.0</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1203,28 +1203,28 @@
                   <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="2">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
                   <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="4">
                   <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>1.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>1.0</c:v>
@@ -1239,7 +1239,7 @@
                   <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>2.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>2.0</c:v>
@@ -1248,166 +1248,166 @@
                   <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="17">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>2.0</c:v>
+                </c:pt>
+                <c:pt idx="23">
                   <c:v>3.0</c:v>
                 </c:pt>
-                <c:pt idx="18">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>6.0</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="22">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="23">
-                  <c:v>5.0</c:v>
-                </c:pt>
                 <c:pt idx="24">
-                  <c:v>6.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>6.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>3.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>4.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>5.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>6.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="30">
                   <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>3.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>3.0</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>3.0</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="34">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="35">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="36">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="37">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="38">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="39">
+                  <c:v>8.0</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="41">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="42">
+                  <c:v>6.0</c:v>
+                </c:pt>
+                <c:pt idx="43">
+                  <c:v>7.0</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>5.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
                   <c:v>2.0</c:v>
                 </c:pt>
-                <c:pt idx="35">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="36">
+                <c:pt idx="48">
                   <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="37">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="38">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="39">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="41">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="42">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="43">
-                  <c:v>4.0</c:v>
-                </c:pt>
-                <c:pt idx="44">
-                  <c:v>5.0</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>6.0</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="49">
                   <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>2.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>2.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>2.0</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>2.0</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>2.0</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>2.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>2.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>1.0</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>2.0</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>1.0</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>1.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>2.0</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>2.0</c:v>
+                  <c:v>6.0</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>2.0</c:v>
+                  <c:v>7.0</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>2.0</c:v>
+                  <c:v>8.0</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>3.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>4.0</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="68">
                   <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>5.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>5.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="71">
                   <c:v>2.0</c:v>
@@ -1451,220 +1451,220 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="72"/>
                 <c:pt idx="0">
-                  <c:v>0.000233</c:v>
+                  <c:v>0.00022</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.00278</c:v>
+                  <c:v>0.002893</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.025366</c:v>
+                  <c:v>0.018636</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.16172</c:v>
+                  <c:v>0.125582</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.693186</c:v>
+                  <c:v>0.696009</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.915595</c:v>
+                  <c:v>1.433526</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.933415</c:v>
+                  <c:v>1.94924</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.068254</c:v>
+                  <c:v>1.433534</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.646653</c:v>
+                  <c:v>0.653106</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.203365</c:v>
+                  <c:v>0.197281</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.033091</c:v>
+                  <c:v>0.020519</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.002535</c:v>
+                  <c:v>0.002003</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.000129</c:v>
+                  <c:v>0.00014</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.001997</c:v>
+                  <c:v>0.003152</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.022188</c:v>
+                  <c:v>0.030667</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.129919</c:v>
+                  <c:v>0.132008</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.397389</c:v>
+                  <c:v>0.710414</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.081538</c:v>
+                  <c:v>1.217522</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.570756</c:v>
+                  <c:v>1.557452</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>1.260968</c:v>
+                  <c:v>0.942168</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.617635</c:v>
+                  <c:v>0.648444</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.154749</c:v>
+                  <c:v>0.194881</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.027173</c:v>
+                  <c:v>0.028915</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.002222</c:v>
+                  <c:v>0.003444</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.000131</c:v>
+                  <c:v>0.000203</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.003744</c:v>
+                  <c:v>0.002519</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.028591</c:v>
+                  <c:v>0.020574</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.174805</c:v>
+                  <c:v>0.116393</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.685385</c:v>
+                  <c:v>0.397213</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>1.009343</c:v>
+                  <c:v>0.807444</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.135428</c:v>
+                  <c:v>1.436517</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1.29198</c:v>
+                  <c:v>1.026869</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.434452</c:v>
+                  <c:v>0.674214</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.210125</c:v>
+                  <c:v>0.176554</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.022914</c:v>
+                  <c:v>0.018511</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.003415</c:v>
+                  <c:v>0.002002</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.000225</c:v>
+                  <c:v>0.000239</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.002092</c:v>
+                  <c:v>0.00215</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.034804</c:v>
+                  <c:v>0.029766</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.133562</c:v>
+                  <c:v>0.107856</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.466909</c:v>
+                  <c:v>0.70229</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>0.838116</c:v>
+                  <c:v>1.085511</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1.088128</c:v>
+                  <c:v>1.579447</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1.514685</c:v>
+                  <c:v>1.10055</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.660235</c:v>
+                  <c:v>0.494708</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.107363</c:v>
+                  <c:v>0.112471</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.022166</c:v>
+                  <c:v>0.020219</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.002463</c:v>
+                  <c:v>0.003258</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.000243</c:v>
+                  <c:v>0.000201</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.003243</c:v>
+                  <c:v>0.003122</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.024998</c:v>
+                  <c:v>0.034438</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.172103</c:v>
+                  <c:v>0.110836</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.69296</c:v>
+                  <c:v>0.419506</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>1.512142</c:v>
+                  <c:v>1.272573</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>1.611818</c:v>
+                  <c:v>1.966645</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>1.312943</c:v>
+                  <c:v>1.185545</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.590105</c:v>
+                  <c:v>0.607645</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.124412</c:v>
+                  <c:v>0.20645</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.024756</c:v>
+                  <c:v>0.031144</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.001982</c:v>
+                  <c:v>0.002254</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.000193</c:v>
+                  <c:v>0.000206</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.003443</c:v>
+                  <c:v>0.003266</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.028778</c:v>
+                  <c:v>0.019204</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.193283</c:v>
+                  <c:v>0.179864</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.703897</c:v>
+                  <c:v>0.384425</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>1.241266</c:v>
+                  <c:v>1.370342</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>1.916276</c:v>
+                  <c:v>1.561923</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>1.01948</c:v>
+                  <c:v>1.459896</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.595708</c:v>
+                  <c:v>0.650755</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.120596</c:v>
+                  <c:v>0.114098</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.024047</c:v>
+                  <c:v>0.022356</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.003678</c:v>
+                  <c:v>0.003281</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1681,11 +1681,11 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="604013184"/>
-        <c:axId val="604015664"/>
+        <c:axId val="-1616447680"/>
+        <c:axId val="-1616445632"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="604013184"/>
+        <c:axId val="-1616447680"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1727,7 +1727,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="604015664"/>
+        <c:crossAx val="-1616445632"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1735,7 +1735,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="604015664"/>
+        <c:axId val="-1616445632"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1786,7 +1786,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="604013184"/>
+        <c:crossAx val="-1616447680"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -2711,7 +2711,7 @@
   <dimension ref="A1:G73"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H12" sqref="H12"/>
+      <selection activeCell="A5" sqref="A5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2744,13 +2744,13 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>32.189883999999999</v>
+        <v>20.885608999999999</v>
       </c>
       <c r="C2">
-        <v>5.8910799999999997</v>
+        <v>7.6922100000000002</v>
       </c>
       <c r="D2">
-        <v>2.6716099999999998</v>
+        <v>0</v>
       </c>
       <c r="E2">
         <v>36</v>
@@ -2759,7 +2759,7 @@
         <v>5</v>
       </c>
       <c r="G2">
-        <v>2.33E-4</v>
+        <v>2.2000000000000001E-4</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -2767,22 +2767,22 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>27.234589</v>
+        <v>44.223166999999997</v>
       </c>
       <c r="C3">
-        <v>11.964765999999999</v>
+        <v>9.3691949999999995</v>
       </c>
       <c r="D3">
-        <v>2.3801260000000002</v>
+        <v>4.8663860000000003</v>
       </c>
       <c r="E3">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="F3">
         <v>5</v>
       </c>
       <c r="G3">
-        <v>2.7799999999999999E-3</v>
+        <v>2.8930000000000002E-3</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -2790,22 +2790,22 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>54.019173000000002</v>
+        <v>44.351357</v>
       </c>
       <c r="C4">
-        <v>13.729722000000001</v>
+        <v>12.331645999999999</v>
       </c>
       <c r="D4">
-        <v>2.002618</v>
+        <v>9.5832189999999997</v>
       </c>
       <c r="E4">
-        <v>21</v>
+        <v>26</v>
       </c>
       <c r="F4">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G4">
-        <v>2.5366E-2</v>
+        <v>1.8636E-2</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -2813,22 +2813,22 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>58.216586999999997</v>
+        <v>56.799408</v>
       </c>
       <c r="C5">
-        <v>11.146072</v>
+        <v>11.443724</v>
       </c>
       <c r="D5">
-        <v>1.2131460000000001</v>
+        <v>8.7305670000000006</v>
       </c>
       <c r="E5">
-        <v>15</v>
+        <v>28</v>
       </c>
       <c r="F5">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G5">
-        <v>0.16172</v>
+        <v>0.125582</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -2836,22 +2836,22 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>70.501082999999994</v>
+        <v>59.47784</v>
       </c>
       <c r="C6">
-        <v>9.2055450000000008</v>
+        <v>11.681658000000001</v>
       </c>
       <c r="D6">
-        <v>0.302151</v>
+        <v>7.3800330000000001</v>
       </c>
       <c r="E6">
-        <v>11</v>
+        <v>28</v>
       </c>
       <c r="F6">
         <v>2</v>
       </c>
       <c r="G6">
-        <v>0.69318599999999997</v>
+        <v>0.69600899999999999</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -2859,22 +2859,22 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>79.072638999999995</v>
+        <v>78.363449000000003</v>
       </c>
       <c r="C7">
-        <v>7.0735140000000003</v>
+        <v>7.2050460000000003</v>
       </c>
       <c r="D7">
-        <v>0</v>
+        <v>5.284027</v>
       </c>
       <c r="E7">
-        <v>9</v>
+        <v>27</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G7">
-        <v>0.91559500000000005</v>
+        <v>1.4335260000000001</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -2882,22 +2882,22 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>61.173186999999999</v>
+        <v>66.634429999999995</v>
       </c>
       <c r="C8">
-        <v>4.7499200000000004</v>
+        <v>6.1645719999999997</v>
       </c>
       <c r="D8">
-        <v>0</v>
+        <v>2.5062329999999999</v>
       </c>
       <c r="E8">
-        <v>8</v>
+        <v>23</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G8">
-        <v>1.9334150000000001</v>
+        <v>1.9492400000000001</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -2905,22 +2905,22 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>72.406998000000002</v>
+        <v>71.832252999999994</v>
       </c>
       <c r="C9">
-        <v>3.2766959999999998</v>
+        <v>3.310365</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>7</v>
+        <v>18</v>
       </c>
       <c r="F9">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G9">
-        <v>1.068254</v>
+        <v>1.4335340000000001</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -2928,7 +2928,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>56.750647999999998</v>
+        <v>55.859355999999998</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -2937,13 +2937,13 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="G10">
-        <v>0.64665300000000003</v>
+        <v>0.65310599999999996</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -2951,22 +2951,22 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>36.692860000000003</v>
+        <v>52.973492</v>
       </c>
       <c r="C11">
-        <v>1.4685440000000001</v>
+        <v>0</v>
       </c>
       <c r="D11">
-        <v>2.5166140000000001</v>
+        <v>0</v>
       </c>
       <c r="E11">
-        <v>5</v>
+        <v>13</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G11">
-        <v>0.20336499999999999</v>
+        <v>0.19728100000000001</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -2974,22 +2974,22 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>36.807288999999997</v>
+        <v>36.075629999999997</v>
       </c>
       <c r="C12">
-        <v>1.1484000000000001</v>
+        <v>1.747986</v>
       </c>
       <c r="D12">
-        <v>5.3635029999999997</v>
+        <v>2.6238389999999998</v>
       </c>
       <c r="E12">
-        <v>4</v>
+        <v>11</v>
       </c>
       <c r="F12">
         <v>1</v>
       </c>
       <c r="G12">
-        <v>3.3091000000000002E-2</v>
+        <v>2.0518999999999999E-2</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -2997,22 +2997,22 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>25.537154999999998</v>
+        <v>22.409046</v>
       </c>
       <c r="C13">
-        <v>4.3049590000000002</v>
+        <v>5.4770240000000001</v>
       </c>
       <c r="D13">
-        <v>5.8445830000000001</v>
+        <v>2.3486829999999999</v>
       </c>
       <c r="E13">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="F13">
         <v>1</v>
       </c>
       <c r="G13">
-        <v>2.5349999999999999E-3</v>
+        <v>2.003E-3</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -3020,22 +3020,22 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>36.750442999999997</v>
+        <v>28.810452000000002</v>
       </c>
       <c r="C14">
-        <v>7.7536750000000003</v>
+        <v>6.2662209999999998</v>
       </c>
       <c r="D14">
-        <v>12.386138000000001</v>
+        <v>3.8863539999999999</v>
       </c>
       <c r="E14">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="F14">
         <v>1</v>
       </c>
       <c r="G14">
-        <v>1.2899999999999999E-4</v>
+        <v>1.3999999999999999E-4</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -3043,22 +3043,22 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>34.712333999999998</v>
+        <v>35.202601999999999</v>
       </c>
       <c r="C15">
-        <v>11.657178999999999</v>
+        <v>11.650181</v>
       </c>
       <c r="D15">
-        <v>17.87088</v>
+        <v>9.7208020000000008</v>
       </c>
       <c r="E15">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="F15">
         <v>1</v>
       </c>
       <c r="G15">
-        <v>1.9970000000000001E-3</v>
+        <v>3.1519999999999999E-3</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -3066,22 +3066,22 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>42.515759000000003</v>
+        <v>36.033852000000003</v>
       </c>
       <c r="C16">
-        <v>10.162119000000001</v>
+        <v>9.8823460000000001</v>
       </c>
       <c r="D16">
-        <v>24.526275999999999</v>
+        <v>16.252264</v>
       </c>
       <c r="E16">
-        <v>27</v>
+        <v>13</v>
       </c>
       <c r="F16">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G16">
-        <v>2.2187999999999999E-2</v>
+        <v>3.0667E-2</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -3089,22 +3089,22 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>58.046599999999998</v>
+        <v>57.877426</v>
       </c>
       <c r="C17">
-        <v>11.768836</v>
+        <v>11.109354</v>
       </c>
       <c r="D17">
-        <v>23.452687999999998</v>
+        <v>15.89499</v>
       </c>
       <c r="E17">
-        <v>34</v>
+        <v>23</v>
       </c>
       <c r="F17">
         <v>2</v>
       </c>
       <c r="G17">
-        <v>0.12991900000000001</v>
+        <v>0.13200799999999999</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -3112,22 +3112,22 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>70.682129000000003</v>
+        <v>73.272002999999998</v>
       </c>
       <c r="C18">
-        <v>9.7922530000000005</v>
+        <v>11.389172</v>
       </c>
       <c r="D18">
-        <v>21.623422999999999</v>
+        <v>14.613104999999999</v>
       </c>
       <c r="E18">
-        <v>39</v>
+        <v>30</v>
       </c>
       <c r="F18">
         <v>2</v>
       </c>
       <c r="G18">
-        <v>0.39738899999999999</v>
+        <v>0.71041399999999999</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -3135,22 +3135,22 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>62.826061000000003</v>
+        <v>61.035522</v>
       </c>
       <c r="C19">
-        <v>7.8318209999999997</v>
+        <v>9.1153759999999995</v>
       </c>
       <c r="D19">
-        <v>19.317709000000001</v>
+        <v>12.497744000000001</v>
       </c>
       <c r="E19">
-        <v>43</v>
+        <v>35</v>
       </c>
       <c r="F19">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G19">
-        <v>1.0815380000000001</v>
+        <v>1.217522</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -3158,22 +3158,22 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>64.542869999999994</v>
+        <v>76.676070999999993</v>
       </c>
       <c r="C20">
-        <v>3.5976919999999999</v>
+        <v>4.1617389999999999</v>
       </c>
       <c r="D20">
-        <v>16.099025999999999</v>
+        <v>9.5302310000000006</v>
       </c>
       <c r="E20">
-        <v>46</v>
+        <v>37</v>
       </c>
       <c r="F20">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G20">
-        <v>1.570756</v>
+        <v>1.5574520000000001</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -3181,22 +3181,22 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>68.095366999999996</v>
+        <v>56.042228999999999</v>
       </c>
       <c r="C21">
-        <v>2.1619799999999998</v>
+        <v>2.749495</v>
       </c>
       <c r="D21">
-        <v>12.229884999999999</v>
+        <v>6.4834490000000002</v>
       </c>
       <c r="E21">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="F21">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G21">
-        <v>1.2609680000000001</v>
+        <v>0.94216800000000001</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -3204,22 +3204,22 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>54.340781999999997</v>
+        <v>56.298614999999998</v>
       </c>
       <c r="C22">
-        <v>0</v>
+        <v>0.50295400000000001</v>
       </c>
       <c r="D22">
-        <v>8.9453040000000001</v>
+        <v>3.96916</v>
       </c>
       <c r="E22">
-        <v>47</v>
+        <v>31</v>
       </c>
       <c r="F22">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G22">
-        <v>0.61763500000000005</v>
+        <v>0.64844400000000002</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -3227,22 +3227,22 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>41.606369000000001</v>
+        <v>52.726635000000002</v>
       </c>
       <c r="C23">
-        <v>1.7468900000000001</v>
+        <v>1.4104540000000001</v>
       </c>
       <c r="D23">
-        <v>9.9228670000000001</v>
+        <v>2.527987</v>
       </c>
       <c r="E23">
-        <v>43</v>
+        <v>24</v>
       </c>
       <c r="F23">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G23">
-        <v>0.154749</v>
+        <v>0.194881</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -3250,22 +3250,22 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>32.098640000000003</v>
+        <v>39.937725</v>
       </c>
       <c r="C24">
-        <v>1.5043660000000001</v>
+        <v>0</v>
       </c>
       <c r="D24">
-        <v>9.7002000000000006</v>
+        <v>4.0760269999999998</v>
       </c>
       <c r="E24">
-        <v>41</v>
+        <v>18</v>
       </c>
       <c r="F24">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G24">
-        <v>2.7172999999999999E-2</v>
+        <v>2.8915E-2</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -3273,22 +3273,22 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>28.382577999999999</v>
+        <v>29.505065999999999</v>
       </c>
       <c r="C25">
-        <v>4.903003</v>
+        <v>6.0307789999999999</v>
       </c>
       <c r="D25">
-        <v>9.2230260000000008</v>
+        <v>5.4186529999999999</v>
       </c>
       <c r="E25">
-        <v>39</v>
+        <v>15</v>
       </c>
       <c r="F25">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G25">
-        <v>2.222E-3</v>
+        <v>3.444E-3</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -3296,22 +3296,22 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>39.996581999999997</v>
+        <v>40.043242999999997</v>
       </c>
       <c r="C26">
-        <v>7.3271879999999996</v>
+        <v>8.1838759999999997</v>
       </c>
       <c r="D26">
-        <v>14.719226000000001</v>
+        <v>12.405503</v>
       </c>
       <c r="E26">
-        <v>37</v>
+        <v>15</v>
       </c>
       <c r="F26">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G26">
-        <v>1.3100000000000001E-4</v>
+        <v>2.03E-4</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -3319,22 +3319,22 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>27.974194000000001</v>
+        <v>44.441383000000002</v>
       </c>
       <c r="C27">
-        <v>10.088284</v>
+        <v>10.889704999999999</v>
       </c>
       <c r="D27">
-        <v>14.752654</v>
+        <v>18.171339</v>
       </c>
       <c r="E27">
-        <v>40</v>
+        <v>22</v>
       </c>
       <c r="F27">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G27">
-        <v>3.7439999999999999E-3</v>
+        <v>2.519E-3</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -3342,22 +3342,22 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>53.898345999999997</v>
+        <v>37.164771999999999</v>
       </c>
       <c r="C28">
-        <v>11.598509</v>
+        <v>11.372070000000001</v>
       </c>
       <c r="D28">
-        <v>13.878945</v>
+        <v>24.313231999999999</v>
       </c>
       <c r="E28">
-        <v>42</v>
+        <v>30</v>
       </c>
       <c r="F28">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="G28">
-        <v>2.8590999999999998E-2</v>
+        <v>2.0573999999999999E-2</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -3365,22 +3365,22 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>62.485992000000003</v>
+        <v>53.447513999999998</v>
       </c>
       <c r="C29">
-        <v>10.287411000000001</v>
+        <v>12.344517</v>
       </c>
       <c r="D29">
-        <v>11.801270000000001</v>
+        <v>24.033906999999999</v>
       </c>
       <c r="E29">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="F29">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G29">
-        <v>0.17480499999999999</v>
+        <v>0.116393</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -3388,22 +3388,22 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>64.313537999999994</v>
+        <v>56.336689</v>
       </c>
       <c r="C30">
-        <v>10.366960000000001</v>
+        <v>8.9871099999999995</v>
       </c>
       <c r="D30">
-        <v>9.4481000000000002</v>
+        <v>22.666494</v>
       </c>
       <c r="E30">
-        <v>44</v>
+        <v>41</v>
       </c>
       <c r="F30">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G30">
-        <v>0.68538500000000002</v>
+        <v>0.39721299999999998</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -3411,22 +3411,22 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>71.178352000000004</v>
+        <v>61.941589</v>
       </c>
       <c r="C31">
-        <v>7.2037240000000002</v>
+        <v>6.7357620000000002</v>
       </c>
       <c r="D31">
-        <v>6.5631589999999997</v>
+        <v>20.277622000000001</v>
       </c>
       <c r="E31">
-        <v>41</v>
+        <v>45</v>
       </c>
       <c r="F31">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G31">
-        <v>1.0093430000000001</v>
+        <v>0.80744400000000005</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -3434,22 +3434,22 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>64.037422000000007</v>
+        <v>62.202953000000001</v>
       </c>
       <c r="C32">
-        <v>4.6007429999999996</v>
+        <v>6.2127629999999998</v>
       </c>
       <c r="D32">
-        <v>3.522316</v>
+        <v>17.270281000000001</v>
       </c>
       <c r="E32">
-        <v>35</v>
+        <v>48</v>
       </c>
       <c r="F32">
         <v>3</v>
       </c>
       <c r="G32">
-        <v>1.1354280000000001</v>
+        <v>1.436517</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -3457,22 +3457,22 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>56.947268999999999</v>
+        <v>65.092360999999997</v>
       </c>
       <c r="C33">
-        <v>0.88562200000000002</v>
+        <v>0</v>
       </c>
       <c r="D33">
-        <v>0.83411900000000005</v>
+        <v>13.439188</v>
       </c>
       <c r="E33">
-        <v>27</v>
+        <v>49</v>
       </c>
       <c r="F33">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G33">
-        <v>1.2919799999999999</v>
+        <v>1.026869</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -3480,22 +3480,22 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>59.490402000000003</v>
+        <v>54.192946999999997</v>
       </c>
       <c r="C34">
-        <v>1.349844</v>
+        <v>0</v>
       </c>
       <c r="D34">
-        <v>0</v>
+        <v>10.354922</v>
       </c>
       <c r="E34">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="F34">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G34">
-        <v>0.434452</v>
+        <v>0.67421399999999998</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -3503,22 +3503,22 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>43.007148999999998</v>
+        <v>39.656619999999997</v>
       </c>
       <c r="C35">
         <v>0</v>
       </c>
       <c r="D35">
-        <v>1.0541259999999999</v>
+        <v>10.220276</v>
       </c>
       <c r="E35">
-        <v>21</v>
+        <v>45</v>
       </c>
       <c r="F35">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G35">
-        <v>0.21012500000000001</v>
+        <v>0.17655399999999999</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -3526,22 +3526,22 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>37.618586999999998</v>
+        <v>33.540306000000001</v>
       </c>
       <c r="C36">
-        <v>0.241978</v>
+        <v>3.5110350000000001</v>
       </c>
       <c r="D36">
-        <v>2.7109559999999999</v>
+        <v>11.253133</v>
       </c>
       <c r="E36">
-        <v>15</v>
+        <v>42</v>
       </c>
       <c r="F36">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G36">
-        <v>2.2914E-2</v>
+        <v>1.8511E-2</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -3549,22 +3549,22 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>25.979164000000001</v>
+        <v>40.206386999999999</v>
       </c>
       <c r="C37">
-        <v>6.0798059999999996</v>
+        <v>5.4708379999999996</v>
       </c>
       <c r="D37">
-        <v>2.8987590000000001</v>
+        <v>15.648156999999999</v>
       </c>
       <c r="E37">
-        <v>12</v>
+        <v>42</v>
       </c>
       <c r="F37">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G37">
-        <v>3.4150000000000001E-3</v>
+        <v>2.0019999999999999E-3</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -3572,22 +3572,22 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>29.115444</v>
+        <v>25.644943000000001</v>
       </c>
       <c r="C38">
-        <v>7.4823040000000001</v>
+        <v>5.740437</v>
       </c>
       <c r="D38">
-        <v>4.5916880000000004</v>
+        <v>14.396024000000001</v>
       </c>
       <c r="E38">
-        <v>9</v>
+        <v>45</v>
       </c>
       <c r="F38">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G38">
-        <v>2.2499999999999999E-4</v>
+        <v>2.3900000000000001E-4</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -3595,22 +3595,22 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>39.134174000000002</v>
+        <v>32.132747999999999</v>
       </c>
       <c r="C39">
-        <v>11.21571</v>
+        <v>8.6201310000000007</v>
       </c>
       <c r="D39">
-        <v>11.965223999999999</v>
+        <v>16.372667</v>
       </c>
       <c r="E39">
-        <v>9</v>
+        <v>46</v>
       </c>
       <c r="F39">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="G39">
-        <v>2.0920000000000001E-3</v>
+        <v>2.15E-3</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -3618,22 +3618,22 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>47.337043999999999</v>
+        <v>44.887669000000002</v>
       </c>
       <c r="C40">
-        <v>12.464180000000001</v>
+        <v>11.138714</v>
       </c>
       <c r="D40">
-        <v>15.907825000000001</v>
+        <v>20.289346999999999</v>
       </c>
       <c r="E40">
-        <v>18</v>
+        <v>48</v>
       </c>
       <c r="F40">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G40">
-        <v>3.4804000000000002E-2</v>
+        <v>2.9766000000000001E-2</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -3641,22 +3641,22 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>48.110329</v>
+        <v>52.063442000000002</v>
       </c>
       <c r="C41">
-        <v>11.959955000000001</v>
+        <v>11.950139</v>
       </c>
       <c r="D41">
-        <v>18.960872999999999</v>
+        <v>19.656628000000001</v>
       </c>
       <c r="E41">
-        <v>27</v>
+        <v>50</v>
       </c>
       <c r="F41">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G41">
-        <v>0.13356199999999999</v>
+        <v>0.10785599999999999</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -3664,22 +3664,22 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>72.052040000000005</v>
+        <v>69.595291000000003</v>
       </c>
       <c r="C42">
-        <v>10.647421</v>
+        <v>8.5272659999999991</v>
       </c>
       <c r="D42">
-        <v>17.477585000000001</v>
+        <v>17.050001000000002</v>
       </c>
       <c r="E42">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="F42">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G42">
-        <v>0.46690900000000002</v>
+        <v>0.70228999999999997</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -3687,22 +3687,22 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>64.318091999999993</v>
+        <v>77.277084000000002</v>
       </c>
       <c r="C43">
-        <v>7.1489339999999997</v>
+        <v>7.4907719999999998</v>
       </c>
       <c r="D43">
-        <v>15.330606</v>
+        <v>13.797719000000001</v>
       </c>
       <c r="E43">
-        <v>39</v>
+        <v>51</v>
       </c>
       <c r="F43">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G43">
-        <v>0.83811599999999997</v>
+        <v>1.0855109999999999</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -3710,22 +3710,22 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>60.346741000000002</v>
+        <v>79.278144999999995</v>
       </c>
       <c r="C44">
-        <v>2.7412649999999998</v>
+        <v>2.7606600000000001</v>
       </c>
       <c r="D44">
-        <v>12.617710000000001</v>
+        <v>10.162209000000001</v>
       </c>
       <c r="E44">
-        <v>42</v>
+        <v>51</v>
       </c>
       <c r="F44">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="G44">
-        <v>1.088128</v>
+        <v>1.579447</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -3733,22 +3733,22 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>57.605164000000002</v>
+        <v>69.433425999999997</v>
       </c>
       <c r="C45">
-        <v>0.37661299999999998</v>
+        <v>0</v>
       </c>
       <c r="D45">
-        <v>9.5724149999999995</v>
+        <v>6.0332699999999999</v>
       </c>
       <c r="E45">
-        <v>42</v>
+        <v>47</v>
       </c>
       <c r="F45">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="G45">
-        <v>1.5146850000000001</v>
+        <v>1.1005499999999999</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
@@ -3756,22 +3756,22 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>61.868670999999999</v>
+        <v>56.146659999999997</v>
       </c>
       <c r="C46">
-        <v>0</v>
+        <v>1.7413860000000001</v>
       </c>
       <c r="D46">
-        <v>5.98238</v>
+        <v>2.8809909999999999</v>
       </c>
       <c r="E46">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="F46">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="G46">
-        <v>0.66023500000000002</v>
+        <v>0.49470799999999998</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -3779,22 +3779,22 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>46.711616999999997</v>
+        <v>40.579189</v>
       </c>
       <c r="C47">
-        <v>0</v>
+        <v>0.95331500000000002</v>
       </c>
       <c r="D47">
-        <v>5.1978479999999996</v>
+        <v>3.9534699999999998</v>
       </c>
       <c r="E47">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="F47">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G47">
-        <v>0.107363</v>
+        <v>0.112471</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -3802,22 +3802,22 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>28.176994000000001</v>
+        <v>39.490268999999998</v>
       </c>
       <c r="C48">
-        <v>3.3099780000000001</v>
+        <v>3.7507220000000001</v>
       </c>
       <c r="D48">
-        <v>4.6541839999999999</v>
+        <v>7.7405099999999996</v>
       </c>
       <c r="E48">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="F48">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G48">
-        <v>2.2166000000000002E-2</v>
+        <v>2.0219000000000001E-2</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -3825,22 +3825,22 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>20.754874999999998</v>
+        <v>36.393768000000001</v>
       </c>
       <c r="C49">
-        <v>5.130077</v>
+        <v>5.7004140000000003</v>
       </c>
       <c r="D49">
-        <v>3.3874629999999999</v>
+        <v>12.359107</v>
       </c>
       <c r="E49">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="F49">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G49">
-        <v>2.4629999999999999E-3</v>
+        <v>3.258E-3</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -3848,22 +3848,22 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>29.549263</v>
+        <v>40.176532999999999</v>
       </c>
       <c r="C50">
-        <v>5.7092720000000003</v>
+        <v>8.2088629999999991</v>
       </c>
       <c r="D50">
-        <v>4.4675820000000002</v>
+        <v>18.900853999999999</v>
       </c>
       <c r="E50">
-        <v>18</v>
+        <v>29</v>
       </c>
       <c r="F50">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G50">
-        <v>2.43E-4</v>
+        <v>2.0100000000000001E-4</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -3871,22 +3871,22 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>31.191721000000001</v>
+        <v>38.817863000000003</v>
       </c>
       <c r="C51">
-        <v>9.5179819999999999</v>
+        <v>12.039536</v>
       </c>
       <c r="D51">
-        <v>7.2412619999999999</v>
+        <v>25.018208000000001</v>
       </c>
       <c r="E51">
-        <v>15</v>
+        <v>36</v>
       </c>
       <c r="F51">
         <v>2</v>
       </c>
       <c r="G51">
-        <v>3.2429999999999998E-3</v>
+        <v>3.1220000000000002E-3</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
@@ -3894,22 +3894,22 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>41.455032000000003</v>
+        <v>36.494812000000003</v>
       </c>
       <c r="C52">
-        <v>12.61899</v>
+        <v>11.336789</v>
       </c>
       <c r="D52">
-        <v>13.801208000000001</v>
+        <v>30.164852</v>
       </c>
       <c r="E52">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="F52">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G52">
-        <v>2.4997999999999999E-2</v>
+        <v>3.4438000000000003E-2</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
@@ -3917,22 +3917,22 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>63.766753999999999</v>
+        <v>49.995823000000001</v>
       </c>
       <c r="C53">
-        <v>11.431450999999999</v>
+        <v>9.8169850000000007</v>
       </c>
       <c r="D53">
-        <v>12.953818</v>
+        <v>31.024920999999999</v>
       </c>
       <c r="E53">
-        <v>25</v>
+        <v>45</v>
       </c>
       <c r="F53">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G53">
-        <v>0.17210300000000001</v>
+        <v>0.110836</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
@@ -3940,22 +3940,22 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>65.617203000000003</v>
+        <v>72.962654000000001</v>
       </c>
       <c r="C54">
-        <v>8.5360630000000004</v>
+        <v>11.537493</v>
       </c>
       <c r="D54">
-        <v>11.542775000000001</v>
+        <v>28.664234</v>
       </c>
       <c r="E54">
-        <v>30</v>
+        <v>48</v>
       </c>
       <c r="F54">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G54">
-        <v>0.69296000000000002</v>
+        <v>0.41950599999999999</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -3963,22 +3963,22 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>72.988219999999998</v>
+        <v>71.332481000000001</v>
       </c>
       <c r="C55">
-        <v>6.8875789999999997</v>
+        <v>9.2917419999999993</v>
       </c>
       <c r="D55">
-        <v>9.3499510000000008</v>
+        <v>25.845161000000001</v>
       </c>
       <c r="E55">
-        <v>33</v>
+        <v>50</v>
       </c>
       <c r="F55">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G55">
-        <v>1.5121420000000001</v>
+        <v>1.272573</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
@@ -3986,22 +3986,22 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>78.380379000000005</v>
+        <v>77.568061999999998</v>
       </c>
       <c r="C56">
-        <v>4.977608</v>
+        <v>2.4539819999999999</v>
       </c>
       <c r="D56">
-        <v>6.187811</v>
+        <v>22.072592</v>
       </c>
       <c r="E56">
-        <v>33</v>
+        <v>51</v>
       </c>
       <c r="F56">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G56">
-        <v>1.611818</v>
+        <v>1.966645</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
@@ -4009,22 +4009,22 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>70.750152999999997</v>
+        <v>62.141407000000001</v>
       </c>
       <c r="C57">
-        <v>1.9854019999999999</v>
+        <v>0.53453899999999999</v>
       </c>
       <c r="D57">
-        <v>2.9263219999999999</v>
+        <v>17.580207999999999</v>
       </c>
       <c r="E57">
-        <v>29</v>
+        <v>52</v>
       </c>
       <c r="F57">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G57">
-        <v>1.312943</v>
+        <v>1.1855450000000001</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
@@ -4032,22 +4032,22 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>47.333176000000002</v>
+        <v>60.944805000000002</v>
       </c>
       <c r="C58">
-        <v>1.1218000000000001E-2</v>
+        <v>2.132727</v>
       </c>
       <c r="D58">
-        <v>1.886142</v>
+        <v>13.848255</v>
       </c>
       <c r="E58">
-        <v>22</v>
+        <v>53</v>
       </c>
       <c r="F58">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G58">
-        <v>0.59010499999999999</v>
+        <v>0.60764499999999999</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
@@ -4055,22 +4055,22 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>47.341106000000003</v>
+        <v>53.533301999999999</v>
       </c>
       <c r="C59">
-        <v>0</v>
+        <v>0.94615000000000005</v>
       </c>
       <c r="D59">
-        <v>1.9129419999999999</v>
+        <v>11.155127999999999</v>
       </c>
       <c r="E59">
-        <v>16</v>
+        <v>52</v>
       </c>
       <c r="F59">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G59">
-        <v>0.12441199999999999</v>
+        <v>0.20644999999999999</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
@@ -4078,22 +4078,22 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>39.534385999999998</v>
+        <v>36.840324000000003</v>
       </c>
       <c r="C60">
-        <v>0</v>
+        <v>0.15592800000000001</v>
       </c>
       <c r="D60">
-        <v>3.925192</v>
+        <v>11.095786</v>
       </c>
       <c r="E60">
-        <v>12</v>
+        <v>49</v>
       </c>
       <c r="F60">
-        <v>1</v>
+        <v>5</v>
       </c>
       <c r="G60">
-        <v>2.4756E-2</v>
+        <v>3.1144000000000002E-2</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
@@ -4101,22 +4101,22 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>21.616539</v>
+        <v>38.933478999999998</v>
       </c>
       <c r="C61">
-        <v>5.5431819999999998</v>
+        <v>2.7077309999999999</v>
       </c>
       <c r="D61">
-        <v>3.5238550000000002</v>
+        <v>13.261982</v>
       </c>
       <c r="E61">
-        <v>10</v>
+        <v>47</v>
       </c>
       <c r="F61">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G61">
-        <v>1.9819999999999998E-3</v>
+        <v>2.2539999999999999E-3</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
@@ -4124,22 +4124,22 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>36.482208</v>
+        <v>25.768913000000001</v>
       </c>
       <c r="C62">
-        <v>6.0940180000000002</v>
+        <v>6.4284290000000004</v>
       </c>
       <c r="D62">
-        <v>9.0904620000000005</v>
+        <v>11.838996</v>
       </c>
       <c r="E62">
-        <v>9</v>
+        <v>47</v>
       </c>
       <c r="F62">
-        <v>1</v>
+        <v>7</v>
       </c>
       <c r="G62">
-        <v>1.93E-4</v>
+        <v>2.0599999999999999E-4</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
@@ -4147,22 +4147,22 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>37.381447000000001</v>
+        <v>42.174145000000003</v>
       </c>
       <c r="C63">
-        <v>11.619752</v>
+        <v>9.7995370000000008</v>
       </c>
       <c r="D63">
-        <v>15.916677999999999</v>
+        <v>17.116368999999999</v>
       </c>
       <c r="E63">
-        <v>15</v>
+        <v>46</v>
       </c>
       <c r="F63">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="G63">
-        <v>3.4429999999999999E-3</v>
+        <v>3.2659999999999998E-3</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
@@ -4170,22 +4170,22 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <v>49.165343999999997</v>
+        <v>50.653114000000002</v>
       </c>
       <c r="C64">
-        <v>10.157206</v>
+        <v>11.142860000000001</v>
       </c>
       <c r="D64">
-        <v>18.615943999999999</v>
+        <v>17.351396999999999</v>
       </c>
       <c r="E64">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="F64">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G64">
-        <v>2.8778000000000001E-2</v>
+        <v>1.9203999999999999E-2</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
@@ -4193,22 +4193,22 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>55.318928</v>
+        <v>59.465423999999999</v>
       </c>
       <c r="C65">
-        <v>10.866258</v>
+        <v>12.895859</v>
       </c>
       <c r="D65">
-        <v>18.146920999999999</v>
+        <v>15.098578</v>
       </c>
       <c r="E65">
-        <v>32</v>
+        <v>50</v>
       </c>
       <c r="F65">
-        <v>2</v>
+        <v>6</v>
       </c>
       <c r="G65">
-        <v>0.19328300000000001</v>
+        <v>0.179864</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
@@ -4216,22 +4216,22 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <v>72.259322999999995</v>
+        <v>57.734195999999997</v>
       </c>
       <c r="C66">
-        <v>11.322286999999999</v>
+        <v>10.564776999999999</v>
       </c>
       <c r="D66">
-        <v>16.353876</v>
+        <v>12.762147000000001</v>
       </c>
       <c r="E66">
-        <v>38</v>
+        <v>50</v>
       </c>
       <c r="F66">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="G66">
-        <v>0.70389699999999999</v>
+        <v>0.38442500000000002</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
@@ -4239,22 +4239,22 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <v>66.098129</v>
+        <v>77.249756000000005</v>
       </c>
       <c r="C67">
-        <v>6.571682</v>
+        <v>7.641038</v>
       </c>
       <c r="D67">
-        <v>13.757814</v>
+        <v>9.8777279999999994</v>
       </c>
       <c r="E67">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="F67">
-        <v>2</v>
+        <v>8</v>
       </c>
       <c r="G67">
-        <v>1.241266</v>
+        <v>1.3703419999999999</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
@@ -4262,22 +4262,22 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <v>64.745018000000002</v>
+        <v>75.877562999999995</v>
       </c>
       <c r="C68">
-        <v>3.0461119999999999</v>
+        <v>4.0006300000000001</v>
       </c>
       <c r="D68">
-        <v>10.427358999999999</v>
+        <v>6.0574000000000003</v>
       </c>
       <c r="E68">
-        <v>43</v>
+        <v>45</v>
       </c>
       <c r="F68">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G68">
-        <v>1.9162760000000001</v>
+        <v>1.561923</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
@@ -4285,22 +4285,22 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <v>71.062507999999994</v>
+        <v>58.825797999999999</v>
       </c>
       <c r="C69">
-        <v>0</v>
+        <v>3.4767269999999999</v>
       </c>
       <c r="D69">
-        <v>6.3612729999999997</v>
+        <v>2.3965200000000002</v>
       </c>
       <c r="E69">
-        <v>42</v>
+        <v>38</v>
       </c>
       <c r="F69">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G69">
-        <v>1.0194799999999999</v>
+        <v>1.4598960000000001</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
@@ -4308,22 +4308,22 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <v>45.309829999999998</v>
+        <v>54.012954999999998</v>
       </c>
       <c r="C70">
+        <v>1.4737420000000001</v>
+      </c>
+      <c r="D70">
         <v>0</v>
       </c>
-      <c r="D70">
-        <v>5.4617740000000001</v>
-      </c>
       <c r="E70">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="F70">
         <v>5</v>
       </c>
       <c r="G70">
-        <v>0.59570800000000002</v>
+        <v>0.65075499999999997</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
@@ -4331,22 +4331,22 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>46.398955999999998</v>
+        <v>44.467818999999999</v>
       </c>
       <c r="C71">
-        <v>0</v>
+        <v>0.15698300000000001</v>
       </c>
       <c r="D71">
-        <v>5.0202549999999997</v>
+        <v>0.38599699999999998</v>
       </c>
       <c r="E71">
-        <v>30</v>
+        <v>24</v>
       </c>
       <c r="F71">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G71">
-        <v>0.12059599999999999</v>
+        <v>0.114098</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
@@ -4354,22 +4354,22 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <v>30.598610000000001</v>
+        <v>28.922798</v>
       </c>
       <c r="C72">
-        <v>3.3735539999999999</v>
+        <v>2.3013590000000002</v>
       </c>
       <c r="D72">
-        <v>5.5304270000000004</v>
+        <v>0.368448</v>
       </c>
       <c r="E72">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="F72">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G72">
-        <v>2.4046999999999999E-2</v>
+        <v>2.2356000000000001E-2</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
@@ -4377,22 +4377,22 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <v>21.391582</v>
+        <v>29.444271000000001</v>
       </c>
       <c r="C73">
-        <v>5.384652</v>
+        <v>5.6954260000000003</v>
       </c>
       <c r="D73">
-        <v>4.4590230000000002</v>
+        <v>1.4273769999999999</v>
       </c>
       <c r="E73">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F73">
         <v>2</v>
       </c>
       <c r="G73">
-        <v>3.6779999999999998E-3</v>
+        <v>3.2810000000000001E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
final version for project 4
</commit_message>
<xml_diff>
--- a/project4/Workbook1.xlsx
+++ b/project4/Workbook1.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>NowPrecip</t>
   </si>
@@ -46,15 +46,34 @@
   <si>
     <t>NowNumPest</t>
   </si>
+  <si>
+    <t>Month</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="10"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="12"/>
+      <color theme="11"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -77,13 +96,21 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="5">
+    <cellStyle name="Followed Hyperlink" xfId="2" builtinId="9" hidden="1"/>
+    <cellStyle name="Followed Hyperlink" xfId="4" builtinId="9" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="1" builtinId="8" hidden="1"/>
+    <cellStyle name="Hyperlink" xfId="3" builtinId="8" hidden="1"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -110,38 +137,7 @@
     </mc:Fallback>
   </mc:AlternateContent>
   <c:chart>
-    <c:title>
-      <c:layout/>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-US"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
+    <c:autoTitleDeleted val="1"/>
     <c:plotArea>
       <c:layout/>
       <c:lineChart>
@@ -150,6 +146,9 @@
         <c:ser>
           <c:idx val="0"/>
           <c:order val="0"/>
+          <c:tx>
+            <c:v>NowTemp</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -181,220 +180,220 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="72"/>
                 <c:pt idx="0">
-                  <c:v>20.885609</c:v>
+                  <c:v>22.29</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>44.223167</c:v>
+                  <c:v>38.54</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>44.351357</c:v>
+                  <c:v>41.33</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>56.799408</c:v>
+                  <c:v>64.62</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>59.47784</c:v>
+                  <c:v>64.8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>78.363449</c:v>
+                  <c:v>74.8</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>66.63443</c:v>
+                  <c:v>68.4</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>71.83225299999999</c:v>
+                  <c:v>57.65</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>55.859356</c:v>
+                  <c:v>47.43</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>52.973492</c:v>
+                  <c:v>46.8</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>36.07563</c:v>
+                  <c:v>33.01</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>22.409046</c:v>
+                  <c:v>34.69</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>28.810452</c:v>
+                  <c:v>26.21</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>35.202602</c:v>
+                  <c:v>35.04</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>36.033852</c:v>
+                  <c:v>37.95</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>57.877426</c:v>
+                  <c:v>53.36</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>73.272003</c:v>
+                  <c:v>61.08</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>61.035522</c:v>
+                  <c:v>77.45</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>76.67607099999999</c:v>
+                  <c:v>67.26</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>56.042229</c:v>
+                  <c:v>61.72</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>56.298615</c:v>
+                  <c:v>56.78</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>52.726635</c:v>
+                  <c:v>48.09</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>39.937725</c:v>
+                  <c:v>30.29</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>29.505066</c:v>
+                  <c:v>35.66</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>40.043243</c:v>
+                  <c:v>31.89</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>44.441383</c:v>
+                  <c:v>38.16</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>37.164772</c:v>
+                  <c:v>47.13</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>53.447514</c:v>
+                  <c:v>56.47</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>56.336689</c:v>
+                  <c:v>67.78</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>61.941589</c:v>
+                  <c:v>77.33</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>62.202953</c:v>
+                  <c:v>63.37</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>65.092361</c:v>
+                  <c:v>55.6</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>54.192947</c:v>
+                  <c:v>56.76</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>39.65662</c:v>
+                  <c:v>36.53</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>33.540306</c:v>
+                  <c:v>42.21</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>40.206387</c:v>
+                  <c:v>20.78</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>25.644943</c:v>
+                  <c:v>33.88</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>32.132748</c:v>
+                  <c:v>30.94</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>44.887669</c:v>
+                  <c:v>45.36</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>52.063442</c:v>
+                  <c:v>46.92</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>69.595291</c:v>
+                  <c:v>67.8</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>77.277084</c:v>
+                  <c:v>76.63</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>79.27814499999999</c:v>
+                  <c:v>61.78</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>69.433426</c:v>
+                  <c:v>56.97</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>56.14666</c:v>
+                  <c:v>57.24</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>40.579189</c:v>
+                  <c:v>35.24</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>39.490269</c:v>
+                  <c:v>45.54</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>36.393768</c:v>
+                  <c:v>39.41</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>40.176533</c:v>
+                  <c:v>26.11</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>38.817863</c:v>
+                  <c:v>27.75</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>36.494812</c:v>
+                  <c:v>35.73</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>49.995823</c:v>
+                  <c:v>54.45</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>72.962654</c:v>
+                  <c:v>57.52</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>71.332481</c:v>
+                  <c:v>74.44</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>77.568062</c:v>
+                  <c:v>77.17</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>62.141407</c:v>
+                  <c:v>68.27</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>60.944805</c:v>
+                  <c:v>63.22</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>53.533302</c:v>
+                  <c:v>45.71</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>36.840324</c:v>
+                  <c:v>41.38</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>38.933479</c:v>
+                  <c:v>29.45</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>25.768913</c:v>
+                  <c:v>29.43</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>42.174145</c:v>
+                  <c:v>28.66</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>50.653114</c:v>
+                  <c:v>48.75</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>59.465424</c:v>
+                  <c:v>46.07</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>57.734196</c:v>
+                  <c:v>72.35</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>77.249756</c:v>
+                  <c:v>76.26</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>75.87756299999999</c:v>
+                  <c:v>65.38</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>58.825798</c:v>
+                  <c:v>72.57</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>54.012955</c:v>
+                  <c:v>60.72</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>44.467819</c:v>
+                  <c:v>43.18</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>28.922798</c:v>
+                  <c:v>37.28</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>29.444271</c:v>
+                  <c:v>22.39</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -404,6 +403,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>NowPrecipitation</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -435,220 +437,220 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="72"/>
                 <c:pt idx="0">
-                  <c:v>7.69221</c:v>
+                  <c:v>5.69</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>9.369195</c:v>
+                  <c:v>10.66</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12.331646</c:v>
+                  <c:v>9.85</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>11.443724</c:v>
+                  <c:v>10.9</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>11.681658</c:v>
+                  <c:v>11.71</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>7.205046</c:v>
+                  <c:v>7.99</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6.164572</c:v>
+                  <c:v>3.66</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>3.310365</c:v>
+                  <c:v>0.72</c:v>
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="9">
+                  <c:v>0.25</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>3.26</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>9.2</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>8.44</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>11.25</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>10.58</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>8.59</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>5.61</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>4.44</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>2.23</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.73</c:v>
+                </c:pt>
+                <c:pt idx="21">
                   <c:v>0.0</c:v>
                 </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.747986</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>5.477024</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>6.266221</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>11.650181</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>9.882346</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>11.109354</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>11.389172</c:v>
-                </c:pt>
-                <c:pt idx="17">
-                  <c:v>9.115376</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>4.161739</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>2.749495</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>0.502954</c:v>
-                </c:pt>
-                <c:pt idx="21">
-                  <c:v>1.410454</c:v>
-                </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.0</c:v>
+                  <c:v>2.21</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>6.030779</c:v>
+                  <c:v>5.39</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>8.183876</c:v>
+                  <c:v>8.99</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>10.889705</c:v>
+                  <c:v>9.96</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>11.37207</c:v>
+                  <c:v>13.07</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>12.344517</c:v>
+                  <c:v>13.49</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>8.98711</c:v>
+                  <c:v>9.45</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>6.735762</c:v>
+                  <c:v>7.29</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>6.212763</c:v>
+                  <c:v>5.36</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>0.0</c:v>
+                  <c:v>1.84</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.0</c:v>
+                  <c:v>1.78</c:v>
                 </c:pt>
                 <c:pt idx="33">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>3.511035</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>5.470838</c:v>
+                  <c:v>6.16</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>5.740437</c:v>
+                  <c:v>9.23</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>8.620131000000001</c:v>
+                  <c:v>8.43</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>11.138714</c:v>
+                  <c:v>13.42</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>11.950139</c:v>
+                  <c:v>11.17</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>8.527266</c:v>
+                  <c:v>9.45</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>7.490772</c:v>
+                  <c:v>7.49</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>2.76066</c:v>
+                  <c:v>3.88</c:v>
                 </c:pt>
                 <c:pt idx="43">
+                  <c:v>2.47</c:v>
+                </c:pt>
+                <c:pt idx="44">
+                  <c:v>0.27</c:v>
+                </c:pt>
+                <c:pt idx="45">
+                  <c:v>1.66</c:v>
+                </c:pt>
+                <c:pt idx="46">
+                  <c:v>0.86</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>5.55</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>5.85</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>11.31</c:v>
+                </c:pt>
+                <c:pt idx="50">
+                  <c:v>11.9</c:v>
+                </c:pt>
+                <c:pt idx="51">
+                  <c:v>12.66</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>10.71</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>6.88</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>4.64</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>2.14</c:v>
+                </c:pt>
+                <c:pt idx="56">
                   <c:v>0.0</c:v>
                 </c:pt>
-                <c:pt idx="44">
-                  <c:v>1.741386</c:v>
-                </c:pt>
-                <c:pt idx="45">
-                  <c:v>0.953315</c:v>
-                </c:pt>
-                <c:pt idx="46">
-                  <c:v>3.750722</c:v>
-                </c:pt>
-                <c:pt idx="47">
-                  <c:v>5.700414</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>8.208863</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>12.039536</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>11.336789</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>9.816985</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>11.537493</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>9.291742</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>2.453982</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>0.534539</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>2.132727</c:v>
-                </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.94615</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.155928</c:v>
+                  <c:v>0.14</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>2.707731</c:v>
+                  <c:v>4.85</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>6.428429</c:v>
+                  <c:v>9.53</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>9.799537</c:v>
+                  <c:v>11.04</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>11.14286</c:v>
+                  <c:v>12.35</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>12.895859</c:v>
+                  <c:v>12.13</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>10.564777</c:v>
+                  <c:v>10.86</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>7.641038</c:v>
+                  <c:v>7.29</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>4.00063</c:v>
+                  <c:v>4.25</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>3.476727</c:v>
+                  <c:v>2.41</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>1.473742</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.156983</c:v>
+                  <c:v>2.13</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>2.301359</c:v>
+                  <c:v>2.96</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>5.695426</c:v>
+                  <c:v>4.45</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -658,6 +660,9 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:v>NowHeight</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -689,25 +694,25 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="72"/>
                 <c:pt idx="0">
+                  <c:v>0.79</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.210000000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>15.77</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>15.42</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>13.71</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>11.14</c:v>
+                </c:pt>
+                <c:pt idx="6">
                   <c:v>0.0</c:v>
-                </c:pt>
-                <c:pt idx="1">
-                  <c:v>4.866386</c:v>
-                </c:pt>
-                <c:pt idx="2">
-                  <c:v>9.583219</c:v>
-                </c:pt>
-                <c:pt idx="3">
-                  <c:v>8.730567000000001</c:v>
-                </c:pt>
-                <c:pt idx="4">
-                  <c:v>7.380033</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>5.284027</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>2.506233</c:v>
                 </c:pt>
                 <c:pt idx="7">
                   <c:v>0.0</c:v>
@@ -719,190 +724,190 @@
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>2.623839</c:v>
+                  <c:v>0.77</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>2.348683</c:v>
+                  <c:v>4.22</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>3.886354</c:v>
+                  <c:v>5.25</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>9.720802000000001</c:v>
+                  <c:v>11.22</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>16.252264</c:v>
+                  <c:v>18.64</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15.89499</c:v>
+                  <c:v>19.54</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>14.613105</c:v>
+                  <c:v>18.52</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>12.497744</c:v>
+                  <c:v>16.97</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>9.530231000000001</c:v>
+                  <c:v>7.9</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>6.483449</c:v>
+                  <c:v>3.28</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>3.96916</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.527987</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>4.076027</c:v>
+                  <c:v>0.74</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>5.418653</c:v>
+                  <c:v>5.82</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>12.405503</c:v>
+                  <c:v>9.76</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>18.171339</c:v>
+                  <c:v>17.34</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>24.313232</c:v>
+                  <c:v>21.5</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>24.033907</c:v>
+                  <c:v>21.6</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>22.666494</c:v>
+                  <c:v>20.32</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>20.277622</c:v>
+                  <c:v>15.03</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>17.270281</c:v>
+                  <c:v>3.63</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>13.439188</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>10.354922</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>10.220276</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>11.253133</c:v>
+                  <c:v>1.61</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>15.648157</c:v>
+                  <c:v>1.43</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>14.396024</c:v>
+                  <c:v>6.73</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>16.372667</c:v>
+                  <c:v>10.05</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>20.289347</c:v>
+                  <c:v>15.25</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>19.656628</c:v>
+                  <c:v>19.85</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>17.050001</c:v>
+                  <c:v>18.54</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>13.797719</c:v>
+                  <c:v>13.31</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>10.162209</c:v>
+                  <c:v>7.64</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>6.03327</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>2.880991</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>3.95347</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>7.740509999999999</c:v>
+                  <c:v>0.57</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>12.359107</c:v>
+                  <c:v>6.65</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>18.900854</c:v>
+                  <c:v>7.42</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>25.018208</c:v>
+                  <c:v>8.97</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>30.164852</c:v>
+                  <c:v>15.19</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>31.024921</c:v>
+                  <c:v>15.58</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>28.664234</c:v>
+                  <c:v>14.38</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>25.845161</c:v>
+                  <c:v>11.57</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>22.072592</c:v>
+                  <c:v>0.92</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>17.580208</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>13.848255</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>11.155128</c:v>
+                  <c:v>1.05</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>11.095786</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>13.261982</c:v>
+                  <c:v>4.6</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>11.838996</c:v>
+                  <c:v>7.06</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>17.116369</c:v>
+                  <c:v>9.140000000000001</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>17.351397</c:v>
+                  <c:v>12.5</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>15.098578</c:v>
+                  <c:v>17.34</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>12.762147</c:v>
+                  <c:v>15.98</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>9.877728</c:v>
+                  <c:v>11.36</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>6.0574</c:v>
+                  <c:v>3.69</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>2.39652</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="68">
                   <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.385997</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.368448</c:v>
+                  <c:v>3.04</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>1.427377</c:v>
+                  <c:v>2.99</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -912,6 +917,9 @@
         <c:ser>
           <c:idx val="3"/>
           <c:order val="3"/>
+          <c:tx>
+            <c:v>NowNumDeer</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -943,73 +951,73 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="72"/>
                 <c:pt idx="0">
+                  <c:v>37.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>33.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>38.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>36.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="8">
                   <c:v>31.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="9">
                   <c:v>26.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="10">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>15.0</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>13.0</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>12.0</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>19.0</c:v>
+                </c:pt>
+                <c:pt idx="15">
                   <c:v>28.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
-                  <c:v>28.0</c:v>
-                </c:pt>
-                <c:pt idx="5">
-                  <c:v>27.0</c:v>
-                </c:pt>
-                <c:pt idx="6">
-                  <c:v>23.0</c:v>
-                </c:pt>
-                <c:pt idx="7">
-                  <c:v>18.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>16.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>11.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>9.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>7.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>6.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>13.0</c:v>
-                </c:pt>
-                <c:pt idx="15">
-                  <c:v>23.0</c:v>
-                </c:pt>
                 <c:pt idx="16">
+                  <c:v>35.0</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>40.0</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>43.0</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="20">
                   <c:v>30.0</c:v>
                 </c:pt>
-                <c:pt idx="17">
-                  <c:v>35.0</c:v>
-                </c:pt>
-                <c:pt idx="18">
-                  <c:v>37.0</c:v>
-                </c:pt>
-                <c:pt idx="19">
-                  <c:v>36.0</c:v>
-                </c:pt>
-                <c:pt idx="20">
-                  <c:v>31.0</c:v>
-                </c:pt>
                 <c:pt idx="21">
-                  <c:v>24.0</c:v>
+                  <c:v>25.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>18.0</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>15.0</c:v>
@@ -1018,10 +1026,10 @@
                   <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>22.0</c:v>
+                  <c:v>20.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>30.0</c:v>
+                  <c:v>29.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
                   <c:v>36.0</c:v>
@@ -1033,130 +1041,130 @@
                   <c:v>45.0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>48.0</c:v>
+                  <c:v>46.0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>49.0</c:v>
+                  <c:v>36.0</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>48.0</c:v>
+                  <c:v>31.0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>45.0</c:v>
+                  <c:v>26.0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>42.0</c:v>
+                  <c:v>21.0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>42.0</c:v>
+                  <c:v>15.0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>45.0</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>46.0</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>48.0</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>50.0</c:v>
+                  <c:v>27.0</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>51.0</c:v>
+                  <c:v>34.0</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>51.0</c:v>
+                  <c:v>39.0</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>51.0</c:v>
+                  <c:v>41.0</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>47.0</c:v>
+                  <c:v>36.0</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>39.0</c:v>
+                  <c:v>33.0</c:v>
                 </c:pt>
                 <c:pt idx="45">
                   <c:v>30.0</c:v>
                 </c:pt>
                 <c:pt idx="46">
+                  <c:v>27.0</c:v>
+                </c:pt>
+                <c:pt idx="47">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>20.0</c:v>
+                </c:pt>
+                <c:pt idx="49">
+                  <c:v>21.0</c:v>
+                </c:pt>
+                <c:pt idx="50">
                   <c:v>24.0</c:v>
                 </c:pt>
-                <c:pt idx="47">
+                <c:pt idx="51">
+                  <c:v>31.0</c:v>
+                </c:pt>
+                <c:pt idx="52">
+                  <c:v>36.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="54">
+                  <c:v>39.0</c:v>
+                </c:pt>
+                <c:pt idx="55">
+                  <c:v>29.0</c:v>
+                </c:pt>
+                <c:pt idx="56">
                   <c:v>24.0</c:v>
                 </c:pt>
-                <c:pt idx="48">
-                  <c:v>29.0</c:v>
-                </c:pt>
-                <c:pt idx="49">
-                  <c:v>36.0</c:v>
-                </c:pt>
-                <c:pt idx="50">
-                  <c:v>41.0</c:v>
-                </c:pt>
-                <c:pt idx="51">
-                  <c:v>45.0</c:v>
-                </c:pt>
-                <c:pt idx="52">
-                  <c:v>48.0</c:v>
-                </c:pt>
-                <c:pt idx="53">
-                  <c:v>50.0</c:v>
-                </c:pt>
-                <c:pt idx="54">
-                  <c:v>51.0</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>52.0</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>53.0</c:v>
-                </c:pt>
                 <c:pt idx="57">
-                  <c:v>52.0</c:v>
+                  <c:v>22.0</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>49.0</c:v>
+                  <c:v>16.0</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>47.0</c:v>
+                  <c:v>12.0</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>47.0</c:v>
+                  <c:v>11.0</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>46.0</c:v>
+                  <c:v>13.0</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>48.0</c:v>
+                  <c:v>18.0</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>50.0</c:v>
+                  <c:v>24.0</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>50.0</c:v>
+                  <c:v>32.0</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>49.0</c:v>
+                  <c:v>37.0</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>45.0</c:v>
+                  <c:v>38.0</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>38.0</c:v>
+                  <c:v>30.0</c:v>
                 </c:pt>
                 <c:pt idx="68">
                   <c:v>29.0</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>24.0</c:v>
+                  <c:v>28.0</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>22.0</c:v>
+                  <c:v>27.0</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>20.0</c:v>
+                  <c:v>21.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1166,6 +1174,9 @@
         <c:ser>
           <c:idx val="4"/>
           <c:order val="4"/>
+          <c:tx>
+            <c:v>NowNumWolf</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -1197,49 +1208,49 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="72"/>
                 <c:pt idx="0">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>4.0</c:v>
+                </c:pt>
+                <c:pt idx="7">
                   <c:v>5.0</c:v>
                 </c:pt>
-                <c:pt idx="1">
+                <c:pt idx="8">
                   <c:v>5.0</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="9">
                   <c:v>5.0</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="10">
                   <c:v>2.0</c:v>
                 </c:pt>
-                <c:pt idx="4">
+                <c:pt idx="11">
                   <c:v>2.0</c:v>
                 </c:pt>
-                <c:pt idx="5">
+                <c:pt idx="12">
                   <c:v>2.0</c:v>
                 </c:pt>
-                <c:pt idx="6">
+                <c:pt idx="13">
                   <c:v>2.0</c:v>
                 </c:pt>
-                <c:pt idx="7">
+                <c:pt idx="14">
                   <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>3.0</c:v>
-                </c:pt>
-                <c:pt idx="9">
-                  <c:v>2.0</c:v>
-                </c:pt>
-                <c:pt idx="10">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="11">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="12">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="13">
-                  <c:v>1.0</c:v>
-                </c:pt>
-                <c:pt idx="14">
-                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="15">
                   <c:v>2.0</c:v>
@@ -1251,166 +1262,166 @@
                   <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>2.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>2.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>2.0</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>2.0</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="22">
                   <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>3.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="24">
                   <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>1.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>2.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>3.0</c:v>
+                  <c:v>4.0</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>4.0</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="32">
                   <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>6.0</c:v>
+                  <c:v>5.0</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>7.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>4.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>5.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>6.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>7.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>8.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>4.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>5.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>6.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>7.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>4.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>5.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>5.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>2.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>2.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>2.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>2.0</c:v>
+                  <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="51">
                   <c:v>3.0</c:v>
                 </c:pt>
                 <c:pt idx="52">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="53">
+                  <c:v>3.0</c:v>
+                </c:pt>
+                <c:pt idx="54">
                   <c:v>4.0</c:v>
                 </c:pt>
-                <c:pt idx="53">
+                <c:pt idx="55">
                   <c:v>5.0</c:v>
                 </c:pt>
-                <c:pt idx="54">
-                  <c:v>6.0</c:v>
-                </c:pt>
-                <c:pt idx="55">
-                  <c:v>7.0</c:v>
-                </c:pt>
                 <c:pt idx="56">
-                  <c:v>8.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>4.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>5.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>6.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>7.0</c:v>
+                  <c:v>2.0</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>4.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>5.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>6.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>7.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>8.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>4.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>5.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>5.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>2.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>2.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>2.0</c:v>
+                  <c:v>1.0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1420,6 +1431,9 @@
         <c:ser>
           <c:idx val="5"/>
           <c:order val="5"/>
+          <c:tx>
+            <c:v>NowNumPest</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
               <a:solidFill>
@@ -1451,220 +1465,220 @@
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="72"/>
                 <c:pt idx="0">
-                  <c:v>0.00022</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.002893</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.018636</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.125582</c:v>
+                  <c:v>0.69</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.696009</c:v>
+                  <c:v>1.1</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>1.433526</c:v>
+                  <c:v>5.52</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>1.94924</c:v>
+                  <c:v>4.82</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>1.433534</c:v>
+                  <c:v>1.13</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.653106</c:v>
+                  <c:v>1.46</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.197281</c:v>
+                  <c:v>0.44</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.020519</c:v>
+                  <c:v>0.09</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.002003</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>0.00014</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>0.003152</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>0.030667</c:v>
+                  <c:v>0.13</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>0.132008</c:v>
+                  <c:v>0.42</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>0.710414</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>1.217522</c:v>
+                  <c:v>4.34</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>1.557452</c:v>
+                  <c:v>2.11</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>0.942168</c:v>
+                  <c:v>2.36</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>0.648444</c:v>
+                  <c:v>1.28</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>0.194881</c:v>
+                  <c:v>0.35</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>0.028915</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>0.003444</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>0.000203</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>0.002519</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>0.020574</c:v>
+                  <c:v>0.04</c:v>
                 </c:pt>
                 <c:pt idx="27">
-                  <c:v>0.116393</c:v>
+                  <c:v>0.46</c:v>
                 </c:pt>
                 <c:pt idx="28">
-                  <c:v>0.397213</c:v>
+                  <c:v>2.44</c:v>
                 </c:pt>
                 <c:pt idx="29">
-                  <c:v>0.807444</c:v>
+                  <c:v>5.49</c:v>
                 </c:pt>
                 <c:pt idx="30">
-                  <c:v>1.436517</c:v>
+                  <c:v>7.93</c:v>
                 </c:pt>
                 <c:pt idx="31">
-                  <c:v>1.026869</c:v>
+                  <c:v>2.06</c:v>
                 </c:pt>
                 <c:pt idx="32">
-                  <c:v>0.674214</c:v>
+                  <c:v>2.43</c:v>
                 </c:pt>
                 <c:pt idx="33">
-                  <c:v>0.176554</c:v>
+                  <c:v>0.47</c:v>
                 </c:pt>
                 <c:pt idx="34">
-                  <c:v>0.018511</c:v>
+                  <c:v>0.07</c:v>
                 </c:pt>
                 <c:pt idx="35">
-                  <c:v>0.002002</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="36">
-                  <c:v>0.000239</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="37">
-                  <c:v>0.00215</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="38">
-                  <c:v>0.029766</c:v>
+                  <c:v>0.05</c:v>
                 </c:pt>
                 <c:pt idx="39">
-                  <c:v>0.107856</c:v>
+                  <c:v>0.52</c:v>
                 </c:pt>
                 <c:pt idx="40">
-                  <c:v>0.70229</c:v>
+                  <c:v>2.44</c:v>
                 </c:pt>
                 <c:pt idx="41">
-                  <c:v>1.085511</c:v>
+                  <c:v>2.67</c:v>
                 </c:pt>
                 <c:pt idx="42">
-                  <c:v>1.579447</c:v>
+                  <c:v>5.71</c:v>
                 </c:pt>
                 <c:pt idx="43">
-                  <c:v>1.10055</c:v>
+                  <c:v>3.09</c:v>
                 </c:pt>
                 <c:pt idx="44">
-                  <c:v>0.494708</c:v>
+                  <c:v>2.8</c:v>
                 </c:pt>
                 <c:pt idx="45">
-                  <c:v>0.112471</c:v>
+                  <c:v>0.84</c:v>
                 </c:pt>
                 <c:pt idx="46">
-                  <c:v>0.020219</c:v>
+                  <c:v>0.1</c:v>
                 </c:pt>
                 <c:pt idx="47">
-                  <c:v>0.003258</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="48">
-                  <c:v>0.000201</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="49">
-                  <c:v>0.003122</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="50">
-                  <c:v>0.034438</c:v>
+                  <c:v>0.15</c:v>
                 </c:pt>
                 <c:pt idx="51">
-                  <c:v>0.110836</c:v>
+                  <c:v>0.63</c:v>
                 </c:pt>
                 <c:pt idx="52">
-                  <c:v>0.419506</c:v>
+                  <c:v>1.22</c:v>
                 </c:pt>
                 <c:pt idx="53">
-                  <c:v>1.272573</c:v>
+                  <c:v>5.13</c:v>
                 </c:pt>
                 <c:pt idx="54">
-                  <c:v>1.966645</c:v>
+                  <c:v>3.85</c:v>
                 </c:pt>
                 <c:pt idx="55">
-                  <c:v>1.185545</c:v>
+                  <c:v>0.91</c:v>
                 </c:pt>
                 <c:pt idx="56">
-                  <c:v>0.607645</c:v>
+                  <c:v>0.42</c:v>
                 </c:pt>
                 <c:pt idx="57">
-                  <c:v>0.20645</c:v>
+                  <c:v>0.4</c:v>
                 </c:pt>
                 <c:pt idx="58">
-                  <c:v>0.031144</c:v>
+                  <c:v>0.13</c:v>
                 </c:pt>
                 <c:pt idx="59">
-                  <c:v>0.002254</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="60">
-                  <c:v>0.000206</c:v>
+                  <c:v>0.0</c:v>
                 </c:pt>
                 <c:pt idx="61">
-                  <c:v>0.003266</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
                 <c:pt idx="62">
-                  <c:v>0.019204</c:v>
+                  <c:v>0.14</c:v>
                 </c:pt>
                 <c:pt idx="63">
-                  <c:v>0.179864</c:v>
+                  <c:v>0.56</c:v>
                 </c:pt>
                 <c:pt idx="64">
-                  <c:v>0.384425</c:v>
+                  <c:v>2.15</c:v>
                 </c:pt>
                 <c:pt idx="65">
-                  <c:v>1.370342</c:v>
+                  <c:v>3.65</c:v>
                 </c:pt>
                 <c:pt idx="66">
-                  <c:v>1.561923</c:v>
+                  <c:v>5.58</c:v>
                 </c:pt>
                 <c:pt idx="67">
-                  <c:v>1.459896</c:v>
+                  <c:v>1.39</c:v>
                 </c:pt>
                 <c:pt idx="68">
-                  <c:v>0.650755</c:v>
+                  <c:v>2.6</c:v>
                 </c:pt>
                 <c:pt idx="69">
-                  <c:v>0.114098</c:v>
+                  <c:v>0.6</c:v>
                 </c:pt>
                 <c:pt idx="70">
-                  <c:v>0.022356</c:v>
+                  <c:v>0.02</c:v>
                 </c:pt>
                 <c:pt idx="71">
-                  <c:v>0.003281</c:v>
+                  <c:v>0.01</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1681,16 +1695,88 @@
         </c:dLbls>
         <c:marker val="1"/>
         <c:smooth val="0"/>
-        <c:axId val="-1616447680"/>
-        <c:axId val="-1616445632"/>
+        <c:axId val="-1616490016"/>
+        <c:axId val="-1616488384"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="-1616447680"/>
+        <c:axId val="-1616490016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="zh-CN" altLang="en-US" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
+                  <a:t>of</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="zh-CN" altLang="en-US" baseline="0"/>
+                  <a:t> </a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN" baseline="0"/>
+                  <a:t>Month</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1727,7 +1813,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1616445632"/>
+        <c:crossAx val="-1616488384"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1735,7 +1821,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="-1616445632"/>
+        <c:axId val="-1616488384"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1755,6 +1841,63 @@
             <a:effectLst/>
           </c:spPr>
         </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US" altLang="zh-CN"/>
+                  <a:t>Quantity</a:t>
+                </a:r>
+                <a:endParaRPr lang="en-US"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:layout/>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
@@ -1786,7 +1929,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-1616447680"/>
+        <c:crossAx val="-1616490016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="between"/>
       </c:valAx>
@@ -1799,7 +1942,7 @@
       </c:spPr>
     </c:plotArea>
     <c:legend>
-      <c:legendPos val="b"/>
+      <c:legendPos val="r"/>
       <c:layout/>
       <c:overlay val="0"/>
       <c:spPr>
@@ -2710,8 +2853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G73"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView tabSelected="1" zoomScale="82" workbookViewId="0">
+      <selection activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2720,6 +2863,9 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>6</v>
+      </c>
       <c r="B1" t="s">
         <v>3</v>
       </c>
@@ -2744,22 +2890,22 @@
         <v>1</v>
       </c>
       <c r="B2">
-        <v>20.885608999999999</v>
+        <v>22.29</v>
       </c>
       <c r="C2">
-        <v>7.6922100000000002</v>
+        <v>5.69</v>
       </c>
       <c r="D2">
+        <v>0.79</v>
+      </c>
+      <c r="E2">
+        <v>37</v>
+      </c>
+      <c r="F2">
+        <v>3</v>
+      </c>
+      <c r="G2">
         <v>0</v>
-      </c>
-      <c r="E2">
-        <v>36</v>
-      </c>
-      <c r="F2">
-        <v>5</v>
-      </c>
-      <c r="G2">
-        <v>2.2000000000000001E-4</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.2">
@@ -2767,22 +2913,22 @@
         <v>2</v>
       </c>
       <c r="B3">
-        <v>44.223166999999997</v>
+        <v>38.54</v>
       </c>
       <c r="C3">
-        <v>9.3691949999999995</v>
+        <v>10.66</v>
       </c>
       <c r="D3">
-        <v>4.8663860000000003</v>
+        <v>8.2100000000000009</v>
       </c>
       <c r="E3">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="F3">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G3">
-        <v>2.8930000000000002E-3</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.2">
@@ -2790,22 +2936,22 @@
         <v>3</v>
       </c>
       <c r="B4">
-        <v>44.351357</v>
+        <v>41.33</v>
       </c>
       <c r="C4">
-        <v>12.331645999999999</v>
+        <v>9.85</v>
       </c>
       <c r="D4">
-        <v>9.5832189999999997</v>
+        <v>15.77</v>
       </c>
       <c r="E4">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="F4">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G4">
-        <v>1.8636E-2</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.2">
@@ -2813,22 +2959,22 @@
         <v>4</v>
       </c>
       <c r="B5">
-        <v>56.799408</v>
+        <v>64.62</v>
       </c>
       <c r="C5">
-        <v>11.443724</v>
+        <v>10.9</v>
       </c>
       <c r="D5">
-        <v>8.7305670000000006</v>
+        <v>15.42</v>
       </c>
       <c r="E5">
-        <v>28</v>
+        <v>33</v>
       </c>
       <c r="F5">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G5">
-        <v>0.125582</v>
+        <v>0.69</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.2">
@@ -2836,22 +2982,22 @@
         <v>5</v>
       </c>
       <c r="B6">
-        <v>59.47784</v>
+        <v>64.8</v>
       </c>
       <c r="C6">
-        <v>11.681658000000001</v>
+        <v>11.71</v>
       </c>
       <c r="D6">
-        <v>7.3800330000000001</v>
+        <v>13.71</v>
       </c>
       <c r="E6">
-        <v>28</v>
+        <v>38</v>
       </c>
       <c r="F6">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G6">
-        <v>0.69600899999999999</v>
+        <v>1.1000000000000001</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.2">
@@ -2859,22 +3005,22 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>78.363449000000003</v>
+        <v>74.8</v>
       </c>
       <c r="C7">
-        <v>7.2050460000000003</v>
+        <v>7.99</v>
       </c>
       <c r="D7">
-        <v>5.284027</v>
+        <v>11.14</v>
       </c>
       <c r="E7">
-        <v>27</v>
+        <v>40</v>
       </c>
       <c r="F7">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G7">
-        <v>1.4335260000000001</v>
+        <v>5.52</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.2">
@@ -2882,22 +3028,22 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>66.634429999999995</v>
+        <v>68.400000000000006</v>
       </c>
       <c r="C8">
-        <v>6.1645719999999997</v>
+        <v>3.66</v>
       </c>
       <c r="D8">
-        <v>2.5062329999999999</v>
+        <v>0</v>
       </c>
       <c r="E8">
-        <v>23</v>
+        <v>40</v>
       </c>
       <c r="F8">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G8">
-        <v>1.9492400000000001</v>
+        <v>4.82</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.2">
@@ -2905,22 +3051,22 @@
         <v>8</v>
       </c>
       <c r="B9">
-        <v>71.832252999999994</v>
+        <v>57.65</v>
       </c>
       <c r="C9">
-        <v>3.310365</v>
+        <v>0.72</v>
       </c>
       <c r="D9">
         <v>0</v>
       </c>
       <c r="E9">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="F9">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G9">
-        <v>1.4335340000000001</v>
+        <v>1.1299999999999999</v>
       </c>
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.2">
@@ -2928,7 +3074,7 @@
         <v>9</v>
       </c>
       <c r="B10">
-        <v>55.859355999999998</v>
+        <v>47.43</v>
       </c>
       <c r="C10">
         <v>0</v>
@@ -2937,13 +3083,13 @@
         <v>0</v>
       </c>
       <c r="E10">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="F10">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="G10">
-        <v>0.65310599999999996</v>
+        <v>1.46</v>
       </c>
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.2">
@@ -2951,22 +3097,22 @@
         <v>10</v>
       </c>
       <c r="B11">
-        <v>52.973492</v>
+        <v>46.8</v>
       </c>
       <c r="C11">
-        <v>0</v>
+        <v>0.25</v>
       </c>
       <c r="D11">
         <v>0</v>
       </c>
       <c r="E11">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="F11">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G11">
-        <v>0.19728100000000001</v>
+        <v>0.44</v>
       </c>
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.2">
@@ -2974,22 +3120,22 @@
         <v>11</v>
       </c>
       <c r="B12">
-        <v>36.075629999999997</v>
+        <v>33.01</v>
       </c>
       <c r="C12">
-        <v>1.747986</v>
+        <v>0.27</v>
       </c>
       <c r="D12">
-        <v>2.6238389999999998</v>
+        <v>0.77</v>
       </c>
       <c r="E12">
-        <v>11</v>
+        <v>21</v>
       </c>
       <c r="F12">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G12">
-        <v>2.0518999999999999E-2</v>
+        <v>0.09</v>
       </c>
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.2">
@@ -2997,22 +3143,22 @@
         <v>12</v>
       </c>
       <c r="B13">
-        <v>22.409046</v>
+        <v>34.69</v>
       </c>
       <c r="C13">
-        <v>5.4770240000000001</v>
+        <v>3.26</v>
       </c>
       <c r="D13">
-        <v>2.3486829999999999</v>
+        <v>4.22</v>
       </c>
       <c r="E13">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="F13">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G13">
-        <v>2.003E-3</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.2">
@@ -3020,22 +3166,22 @@
         <v>13</v>
       </c>
       <c r="B14">
-        <v>28.810452000000002</v>
+        <v>26.21</v>
       </c>
       <c r="C14">
-        <v>6.2662209999999998</v>
+        <v>9.1999999999999993</v>
       </c>
       <c r="D14">
-        <v>3.8863539999999999</v>
+        <v>5.25</v>
       </c>
       <c r="E14">
-        <v>7</v>
+        <v>13</v>
       </c>
       <c r="F14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G14">
-        <v>1.3999999999999999E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.2">
@@ -3043,22 +3189,22 @@
         <v>14</v>
       </c>
       <c r="B15">
-        <v>35.202601999999999</v>
+        <v>35.04</v>
       </c>
       <c r="C15">
-        <v>11.650181</v>
+        <v>8.44</v>
       </c>
       <c r="D15">
-        <v>9.7208020000000008</v>
+        <v>11.22</v>
       </c>
       <c r="E15">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="F15">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G15">
-        <v>3.1519999999999999E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.2">
@@ -3066,22 +3212,22 @@
         <v>15</v>
       </c>
       <c r="B16">
-        <v>36.033852000000003</v>
+        <v>37.950000000000003</v>
       </c>
       <c r="C16">
-        <v>9.8823460000000001</v>
+        <v>11.25</v>
       </c>
       <c r="D16">
-        <v>16.252264</v>
+        <v>18.64</v>
       </c>
       <c r="E16">
-        <v>13</v>
+        <v>19</v>
       </c>
       <c r="F16">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G16">
-        <v>3.0667E-2</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.2">
@@ -3089,22 +3235,22 @@
         <v>16</v>
       </c>
       <c r="B17">
-        <v>57.877426</v>
+        <v>53.36</v>
       </c>
       <c r="C17">
-        <v>11.109354</v>
+        <v>10.58</v>
       </c>
       <c r="D17">
-        <v>15.89499</v>
+        <v>19.54</v>
       </c>
       <c r="E17">
-        <v>23</v>
+        <v>28</v>
       </c>
       <c r="F17">
         <v>2</v>
       </c>
       <c r="G17">
-        <v>0.13200799999999999</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.2">
@@ -3112,22 +3258,22 @@
         <v>17</v>
       </c>
       <c r="B18">
-        <v>73.272002999999998</v>
+        <v>61.08</v>
       </c>
       <c r="C18">
-        <v>11.389172</v>
+        <v>8.59</v>
       </c>
       <c r="D18">
-        <v>14.613104999999999</v>
+        <v>18.52</v>
       </c>
       <c r="E18">
-        <v>30</v>
+        <v>35</v>
       </c>
       <c r="F18">
         <v>2</v>
       </c>
       <c r="G18">
-        <v>0.71041399999999999</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.2">
@@ -3135,22 +3281,22 @@
         <v>18</v>
       </c>
       <c r="B19">
-        <v>61.035522</v>
+        <v>77.45</v>
       </c>
       <c r="C19">
-        <v>9.1153759999999995</v>
+        <v>5.61</v>
       </c>
       <c r="D19">
-        <v>12.497744000000001</v>
+        <v>16.97</v>
       </c>
       <c r="E19">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="F19">
         <v>2</v>
       </c>
       <c r="G19">
-        <v>1.217522</v>
+        <v>4.34</v>
       </c>
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.2">
@@ -3158,22 +3304,22 @@
         <v>19</v>
       </c>
       <c r="B20">
-        <v>76.676070999999993</v>
+        <v>67.260000000000005</v>
       </c>
       <c r="C20">
-        <v>4.1617389999999999</v>
+        <v>4.4400000000000004</v>
       </c>
       <c r="D20">
-        <v>9.5302310000000006</v>
+        <v>7.9</v>
       </c>
       <c r="E20">
-        <v>37</v>
+        <v>43</v>
       </c>
       <c r="F20">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G20">
-        <v>1.5574520000000001</v>
+        <v>2.11</v>
       </c>
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.2">
@@ -3181,22 +3327,22 @@
         <v>20</v>
       </c>
       <c r="B21">
-        <v>56.042228999999999</v>
+        <v>61.72</v>
       </c>
       <c r="C21">
-        <v>2.749495</v>
+        <v>2.23</v>
       </c>
       <c r="D21">
-        <v>6.4834490000000002</v>
+        <v>3.28</v>
       </c>
       <c r="E21">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="F21">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="G21">
-        <v>0.94216800000000001</v>
+        <v>2.36</v>
       </c>
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.2">
@@ -3204,22 +3350,22 @@
         <v>21</v>
       </c>
       <c r="B22">
-        <v>56.298614999999998</v>
+        <v>56.78</v>
       </c>
       <c r="C22">
-        <v>0.50295400000000001</v>
+        <v>0.73</v>
       </c>
       <c r="D22">
-        <v>3.96916</v>
+        <v>0</v>
       </c>
       <c r="E22">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="F22">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G22">
-        <v>0.64844400000000002</v>
+        <v>1.28</v>
       </c>
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.2">
@@ -3227,22 +3373,22 @@
         <v>22</v>
       </c>
       <c r="B23">
-        <v>52.726635000000002</v>
+        <v>48.09</v>
       </c>
       <c r="C23">
-        <v>1.4104540000000001</v>
+        <v>0</v>
       </c>
       <c r="D23">
-        <v>2.527987</v>
+        <v>0</v>
       </c>
       <c r="E23">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="F23">
-        <v>2</v>
+        <v>5</v>
       </c>
       <c r="G23">
-        <v>0.194881</v>
+        <v>0.35</v>
       </c>
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.2">
@@ -3250,22 +3396,22 @@
         <v>23</v>
       </c>
       <c r="B24">
-        <v>39.937725</v>
+        <v>30.29</v>
       </c>
       <c r="C24">
-        <v>0</v>
+        <v>2.21</v>
       </c>
       <c r="D24">
-        <v>4.0760269999999998</v>
+        <v>0.74</v>
       </c>
       <c r="E24">
-        <v>18</v>
+        <v>20</v>
       </c>
       <c r="F24">
         <v>2</v>
       </c>
       <c r="G24">
-        <v>2.8915E-2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.2">
@@ -3273,22 +3419,22 @@
         <v>24</v>
       </c>
       <c r="B25">
-        <v>29.505065999999999</v>
+        <v>35.659999999999997</v>
       </c>
       <c r="C25">
-        <v>6.0307789999999999</v>
+        <v>5.39</v>
       </c>
       <c r="D25">
-        <v>5.4186529999999999</v>
+        <v>5.82</v>
       </c>
       <c r="E25">
         <v>15</v>
       </c>
       <c r="F25">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="G25">
-        <v>3.444E-3</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.2">
@@ -3296,13 +3442,13 @@
         <v>25</v>
       </c>
       <c r="B26">
-        <v>40.043242999999997</v>
+        <v>31.89</v>
       </c>
       <c r="C26">
-        <v>8.1838759999999997</v>
+        <v>8.99</v>
       </c>
       <c r="D26">
-        <v>12.405503</v>
+        <v>9.76</v>
       </c>
       <c r="E26">
         <v>15</v>
@@ -3311,7 +3457,7 @@
         <v>2</v>
       </c>
       <c r="G26">
-        <v>2.03E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.2">
@@ -3319,22 +3465,22 @@
         <v>26</v>
       </c>
       <c r="B27">
-        <v>44.441383000000002</v>
+        <v>38.159999999999997</v>
       </c>
       <c r="C27">
-        <v>10.889704999999999</v>
+        <v>9.9600000000000009</v>
       </c>
       <c r="D27">
-        <v>18.171339</v>
+        <v>17.34</v>
       </c>
       <c r="E27">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="F27">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G27">
-        <v>2.519E-3</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.2">
@@ -3342,22 +3488,22 @@
         <v>27</v>
       </c>
       <c r="B28">
-        <v>37.164771999999999</v>
+        <v>47.13</v>
       </c>
       <c r="C28">
-        <v>11.372070000000001</v>
+        <v>13.07</v>
       </c>
       <c r="D28">
-        <v>24.313231999999999</v>
+        <v>21.5</v>
       </c>
       <c r="E28">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="F28">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G28">
-        <v>2.0573999999999999E-2</v>
+        <v>0.04</v>
       </c>
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.2">
@@ -3365,22 +3511,22 @@
         <v>28</v>
       </c>
       <c r="B29">
-        <v>53.447513999999998</v>
+        <v>56.47</v>
       </c>
       <c r="C29">
-        <v>12.344517</v>
+        <v>13.49</v>
       </c>
       <c r="D29">
-        <v>24.033906999999999</v>
+        <v>21.6</v>
       </c>
       <c r="E29">
         <v>36</v>
       </c>
       <c r="F29">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G29">
-        <v>0.116393</v>
+        <v>0.46</v>
       </c>
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.2">
@@ -3388,22 +3534,22 @@
         <v>29</v>
       </c>
       <c r="B30">
-        <v>56.336689</v>
+        <v>67.78</v>
       </c>
       <c r="C30">
-        <v>8.9871099999999995</v>
+        <v>9.4499999999999993</v>
       </c>
       <c r="D30">
-        <v>22.666494</v>
+        <v>20.32</v>
       </c>
       <c r="E30">
         <v>41</v>
       </c>
       <c r="F30">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="G30">
-        <v>0.39721299999999998</v>
+        <v>2.44</v>
       </c>
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.2">
@@ -3411,22 +3557,22 @@
         <v>30</v>
       </c>
       <c r="B31">
-        <v>61.941589</v>
+        <v>77.33</v>
       </c>
       <c r="C31">
-        <v>6.7357620000000002</v>
+        <v>7.29</v>
       </c>
       <c r="D31">
-        <v>20.277622000000001</v>
+        <v>15.03</v>
       </c>
       <c r="E31">
         <v>45</v>
       </c>
       <c r="F31">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G31">
-        <v>0.80744400000000005</v>
+        <v>5.49</v>
       </c>
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.2">
@@ -3434,22 +3580,22 @@
         <v>31</v>
       </c>
       <c r="B32">
-        <v>62.202953000000001</v>
+        <v>63.37</v>
       </c>
       <c r="C32">
-        <v>6.2127629999999998</v>
+        <v>5.36</v>
       </c>
       <c r="D32">
-        <v>17.270281000000001</v>
+        <v>3.63</v>
       </c>
       <c r="E32">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="F32">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="G32">
-        <v>1.436517</v>
+        <v>7.93</v>
       </c>
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.2">
@@ -3457,22 +3603,22 @@
         <v>32</v>
       </c>
       <c r="B33">
-        <v>65.092360999999997</v>
+        <v>55.6</v>
       </c>
       <c r="C33">
+        <v>1.84</v>
+      </c>
+      <c r="D33">
         <v>0</v>
       </c>
-      <c r="D33">
-        <v>13.439188</v>
-      </c>
       <c r="E33">
-        <v>49</v>
+        <v>36</v>
       </c>
       <c r="F33">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="G33">
-        <v>1.026869</v>
+        <v>2.06</v>
       </c>
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.2">
@@ -3480,22 +3626,22 @@
         <v>33</v>
       </c>
       <c r="B34">
-        <v>54.192946999999997</v>
+        <v>56.76</v>
       </c>
       <c r="C34">
+        <v>1.78</v>
+      </c>
+      <c r="D34">
         <v>0</v>
       </c>
-      <c r="D34">
-        <v>10.354922</v>
-      </c>
       <c r="E34">
-        <v>48</v>
+        <v>31</v>
       </c>
       <c r="F34">
         <v>5</v>
       </c>
       <c r="G34">
-        <v>0.67421399999999998</v>
+        <v>2.4300000000000002</v>
       </c>
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.2">
@@ -3503,22 +3649,22 @@
         <v>34</v>
       </c>
       <c r="B35">
-        <v>39.656619999999997</v>
+        <v>36.53</v>
       </c>
       <c r="C35">
         <v>0</v>
       </c>
       <c r="D35">
-        <v>10.220276</v>
+        <v>0</v>
       </c>
       <c r="E35">
-        <v>45</v>
+        <v>26</v>
       </c>
       <c r="F35">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="G35">
-        <v>0.17655399999999999</v>
+        <v>0.47</v>
       </c>
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.2">
@@ -3526,22 +3672,22 @@
         <v>35</v>
       </c>
       <c r="B36">
-        <v>33.540306000000001</v>
+        <v>42.21</v>
       </c>
       <c r="C36">
-        <v>3.5110350000000001</v>
+        <v>0</v>
       </c>
       <c r="D36">
-        <v>11.253133</v>
+        <v>1.61</v>
       </c>
       <c r="E36">
-        <v>42</v>
+        <v>21</v>
       </c>
       <c r="F36">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G36">
-        <v>1.8511E-2</v>
+        <v>7.0000000000000007E-2</v>
       </c>
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.2">
@@ -3549,22 +3695,22 @@
         <v>36</v>
       </c>
       <c r="B37">
-        <v>40.206386999999999</v>
+        <v>20.78</v>
       </c>
       <c r="C37">
-        <v>5.4708379999999996</v>
+        <v>6.16</v>
       </c>
       <c r="D37">
-        <v>15.648156999999999</v>
+        <v>1.43</v>
       </c>
       <c r="E37">
-        <v>42</v>
+        <v>15</v>
       </c>
       <c r="F37">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G37">
-        <v>2.0019999999999999E-3</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.2">
@@ -3572,22 +3718,22 @@
         <v>37</v>
       </c>
       <c r="B38">
-        <v>25.644943000000001</v>
+        <v>33.880000000000003</v>
       </c>
       <c r="C38">
-        <v>5.740437</v>
+        <v>9.23</v>
       </c>
       <c r="D38">
-        <v>14.396024000000001</v>
+        <v>6.73</v>
       </c>
       <c r="E38">
-        <v>45</v>
+        <v>11</v>
       </c>
       <c r="F38">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G38">
-        <v>2.3900000000000001E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.2">
@@ -3595,22 +3741,22 @@
         <v>38</v>
       </c>
       <c r="B39">
-        <v>32.132747999999999</v>
+        <v>30.94</v>
       </c>
       <c r="C39">
-        <v>8.6201310000000007</v>
+        <v>8.43</v>
       </c>
       <c r="D39">
-        <v>16.372667</v>
+        <v>10.050000000000001</v>
       </c>
       <c r="E39">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="F39">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G39">
-        <v>2.15E-3</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.2">
@@ -3618,22 +3764,22 @@
         <v>39</v>
       </c>
       <c r="B40">
-        <v>44.887669000000002</v>
+        <v>45.36</v>
       </c>
       <c r="C40">
-        <v>11.138714</v>
+        <v>13.42</v>
       </c>
       <c r="D40">
-        <v>20.289346999999999</v>
+        <v>15.25</v>
       </c>
       <c r="E40">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="F40">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G40">
-        <v>2.9766000000000001E-2</v>
+        <v>0.05</v>
       </c>
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.2">
@@ -3641,22 +3787,22 @@
         <v>40</v>
       </c>
       <c r="B41">
-        <v>52.063442000000002</v>
+        <v>46.92</v>
       </c>
       <c r="C41">
-        <v>11.950139</v>
+        <v>11.17</v>
       </c>
       <c r="D41">
-        <v>19.656628000000001</v>
+        <v>19.850000000000001</v>
       </c>
       <c r="E41">
-        <v>50</v>
+        <v>27</v>
       </c>
       <c r="F41">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G41">
-        <v>0.10785599999999999</v>
+        <v>0.52</v>
       </c>
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.2">
@@ -3664,22 +3810,22 @@
         <v>41</v>
       </c>
       <c r="B42">
-        <v>69.595291000000003</v>
+        <v>67.8</v>
       </c>
       <c r="C42">
-        <v>8.5272659999999991</v>
+        <v>9.4499999999999993</v>
       </c>
       <c r="D42">
-        <v>17.050001000000002</v>
+        <v>18.54</v>
       </c>
       <c r="E42">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="F42">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G42">
-        <v>0.70228999999999997</v>
+        <v>2.44</v>
       </c>
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.2">
@@ -3687,22 +3833,22 @@
         <v>42</v>
       </c>
       <c r="B43">
-        <v>77.277084000000002</v>
+        <v>76.63</v>
       </c>
       <c r="C43">
-        <v>7.4907719999999998</v>
+        <v>7.49</v>
       </c>
       <c r="D43">
-        <v>13.797719000000001</v>
+        <v>13.31</v>
       </c>
       <c r="E43">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F43">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G43">
-        <v>1.0855109999999999</v>
+        <v>2.67</v>
       </c>
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.2">
@@ -3710,22 +3856,22 @@
         <v>43</v>
       </c>
       <c r="B44">
-        <v>79.278144999999995</v>
+        <v>61.78</v>
       </c>
       <c r="C44">
-        <v>2.7606600000000001</v>
+        <v>3.88</v>
       </c>
       <c r="D44">
-        <v>10.162209000000001</v>
+        <v>7.64</v>
       </c>
       <c r="E44">
-        <v>51</v>
+        <v>41</v>
       </c>
       <c r="F44">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G44">
-        <v>1.579447</v>
+        <v>5.71</v>
       </c>
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.2">
@@ -3733,22 +3879,22 @@
         <v>44</v>
       </c>
       <c r="B45">
-        <v>69.433425999999997</v>
+        <v>56.97</v>
       </c>
       <c r="C45">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="D45">
         <v>0</v>
       </c>
-      <c r="D45">
-        <v>6.0332699999999999</v>
-      </c>
       <c r="E45">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="F45">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="G45">
-        <v>1.1005499999999999</v>
+        <v>3.09</v>
       </c>
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.2">
@@ -3756,22 +3902,22 @@
         <v>45</v>
       </c>
       <c r="B46">
-        <v>56.146659999999997</v>
+        <v>57.24</v>
       </c>
       <c r="C46">
-        <v>1.7413860000000001</v>
+        <v>0.27</v>
       </c>
       <c r="D46">
-        <v>2.8809909999999999</v>
+        <v>0</v>
       </c>
       <c r="E46">
-        <v>39</v>
+        <v>33</v>
       </c>
       <c r="F46">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G46">
-        <v>0.49470799999999998</v>
+        <v>2.8</v>
       </c>
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.2">
@@ -3779,22 +3925,22 @@
         <v>46</v>
       </c>
       <c r="B47">
-        <v>40.579189</v>
+        <v>35.24</v>
       </c>
       <c r="C47">
-        <v>0.95331500000000002</v>
+        <v>1.66</v>
       </c>
       <c r="D47">
-        <v>3.9534699999999998</v>
+        <v>0</v>
       </c>
       <c r="E47">
         <v>30</v>
       </c>
       <c r="F47">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G47">
-        <v>0.112471</v>
+        <v>0.84</v>
       </c>
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.2">
@@ -3802,22 +3948,22 @@
         <v>47</v>
       </c>
       <c r="B48">
-        <v>39.490268999999998</v>
+        <v>45.54</v>
       </c>
       <c r="C48">
-        <v>3.7507220000000001</v>
+        <v>0.86</v>
       </c>
       <c r="D48">
-        <v>7.7405099999999996</v>
+        <v>0.56999999999999995</v>
       </c>
       <c r="E48">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="F48">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G48">
-        <v>2.0219000000000001E-2</v>
+        <v>0.1</v>
       </c>
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.2">
@@ -3825,22 +3971,22 @@
         <v>48</v>
       </c>
       <c r="B49">
-        <v>36.393768000000001</v>
+        <v>39.409999999999997</v>
       </c>
       <c r="C49">
-        <v>5.7004140000000003</v>
+        <v>5.55</v>
       </c>
       <c r="D49">
-        <v>12.359107</v>
+        <v>6.65</v>
       </c>
       <c r="E49">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="F49">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G49">
-        <v>3.258E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.2">
@@ -3848,22 +3994,22 @@
         <v>49</v>
       </c>
       <c r="B50">
-        <v>40.176532999999999</v>
+        <v>26.11</v>
       </c>
       <c r="C50">
-        <v>8.2088629999999991</v>
+        <v>5.85</v>
       </c>
       <c r="D50">
-        <v>18.900853999999999</v>
+        <v>7.42</v>
       </c>
       <c r="E50">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="F50">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G50">
-        <v>2.0100000000000001E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.2">
@@ -3871,22 +4017,22 @@
         <v>50</v>
       </c>
       <c r="B51">
-        <v>38.817863000000003</v>
+        <v>27.75</v>
       </c>
       <c r="C51">
-        <v>12.039536</v>
+        <v>11.31</v>
       </c>
       <c r="D51">
-        <v>25.018208000000001</v>
+        <v>8.9700000000000006</v>
       </c>
       <c r="E51">
-        <v>36</v>
+        <v>21</v>
       </c>
       <c r="F51">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G51">
-        <v>3.1220000000000002E-3</v>
+        <v>0</v>
       </c>
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.2">
@@ -3894,22 +4040,22 @@
         <v>51</v>
       </c>
       <c r="B52">
-        <v>36.494812000000003</v>
+        <v>35.729999999999997</v>
       </c>
       <c r="C52">
-        <v>11.336789</v>
+        <v>11.9</v>
       </c>
       <c r="D52">
-        <v>30.164852</v>
+        <v>15.19</v>
       </c>
       <c r="E52">
-        <v>41</v>
+        <v>24</v>
       </c>
       <c r="F52">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="G52">
-        <v>3.4438000000000003E-2</v>
+        <v>0.15</v>
       </c>
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.2">
@@ -3917,22 +4063,22 @@
         <v>52</v>
       </c>
       <c r="B53">
-        <v>49.995823000000001</v>
+        <v>54.45</v>
       </c>
       <c r="C53">
-        <v>9.8169850000000007</v>
+        <v>12.66</v>
       </c>
       <c r="D53">
-        <v>31.024920999999999</v>
+        <v>15.58</v>
       </c>
       <c r="E53">
-        <v>45</v>
+        <v>31</v>
       </c>
       <c r="F53">
         <v>3</v>
       </c>
       <c r="G53">
-        <v>0.110836</v>
+        <v>0.63</v>
       </c>
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.2">
@@ -3940,22 +4086,22 @@
         <v>53</v>
       </c>
       <c r="B54">
-        <v>72.962654000000001</v>
+        <v>57.52</v>
       </c>
       <c r="C54">
-        <v>11.537493</v>
+        <v>10.71</v>
       </c>
       <c r="D54">
-        <v>28.664234</v>
+        <v>14.38</v>
       </c>
       <c r="E54">
-        <v>48</v>
+        <v>36</v>
       </c>
       <c r="F54">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="G54">
-        <v>0.41950599999999999</v>
+        <v>1.22</v>
       </c>
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.2">
@@ -3963,22 +4109,22 @@
         <v>54</v>
       </c>
       <c r="B55">
-        <v>71.332481000000001</v>
+        <v>74.44</v>
       </c>
       <c r="C55">
-        <v>9.2917419999999993</v>
+        <v>6.88</v>
       </c>
       <c r="D55">
-        <v>25.845161000000001</v>
+        <v>11.57</v>
       </c>
       <c r="E55">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="F55">
-        <v>5</v>
+        <v>3</v>
       </c>
       <c r="G55">
-        <v>1.272573</v>
+        <v>5.13</v>
       </c>
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.2">
@@ -3986,22 +4132,22 @@
         <v>55</v>
       </c>
       <c r="B56">
-        <v>77.568061999999998</v>
+        <v>77.17</v>
       </c>
       <c r="C56">
-        <v>2.4539819999999999</v>
+        <v>4.6399999999999997</v>
       </c>
       <c r="D56">
-        <v>22.072592</v>
+        <v>0.92</v>
       </c>
       <c r="E56">
-        <v>51</v>
+        <v>39</v>
       </c>
       <c r="F56">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="G56">
-        <v>1.966645</v>
+        <v>3.85</v>
       </c>
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.2">
@@ -4009,22 +4155,22 @@
         <v>56</v>
       </c>
       <c r="B57">
-        <v>62.141407000000001</v>
+        <v>68.27</v>
       </c>
       <c r="C57">
-        <v>0.53453899999999999</v>
+        <v>2.14</v>
       </c>
       <c r="D57">
-        <v>17.580207999999999</v>
+        <v>0</v>
       </c>
       <c r="E57">
-        <v>52</v>
+        <v>29</v>
       </c>
       <c r="F57">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="G57">
-        <v>1.1855450000000001</v>
+        <v>0.91</v>
       </c>
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.2">
@@ -4032,22 +4178,22 @@
         <v>57</v>
       </c>
       <c r="B58">
-        <v>60.944805000000002</v>
+        <v>63.22</v>
       </c>
       <c r="C58">
-        <v>2.132727</v>
+        <v>0</v>
       </c>
       <c r="D58">
-        <v>13.848255</v>
+        <v>0</v>
       </c>
       <c r="E58">
-        <v>53</v>
+        <v>24</v>
       </c>
       <c r="F58">
-        <v>8</v>
+        <v>2</v>
       </c>
       <c r="G58">
-        <v>0.60764499999999999</v>
+        <v>0.42</v>
       </c>
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.2">
@@ -4055,22 +4201,22 @@
         <v>58</v>
       </c>
       <c r="B59">
-        <v>53.533301999999999</v>
+        <v>45.71</v>
       </c>
       <c r="C59">
-        <v>0.94615000000000005</v>
+        <v>0</v>
       </c>
       <c r="D59">
-        <v>11.155127999999999</v>
+        <v>1.05</v>
       </c>
       <c r="E59">
-        <v>52</v>
+        <v>22</v>
       </c>
       <c r="F59">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="G59">
-        <v>0.20644999999999999</v>
+        <v>0.4</v>
       </c>
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.2">
@@ -4078,22 +4224,22 @@
         <v>59</v>
       </c>
       <c r="B60">
-        <v>36.840324000000003</v>
+        <v>41.38</v>
       </c>
       <c r="C60">
-        <v>0.15592800000000001</v>
+        <v>0.14000000000000001</v>
       </c>
       <c r="D60">
-        <v>11.095786</v>
+        <v>3</v>
       </c>
       <c r="E60">
-        <v>49</v>
+        <v>16</v>
       </c>
       <c r="F60">
-        <v>5</v>
+        <v>2</v>
       </c>
       <c r="G60">
-        <v>3.1144000000000002E-2</v>
+        <v>0.13</v>
       </c>
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.2">
@@ -4101,22 +4247,22 @@
         <v>60</v>
       </c>
       <c r="B61">
-        <v>38.933478999999998</v>
+        <v>29.45</v>
       </c>
       <c r="C61">
-        <v>2.7077309999999999</v>
+        <v>4.8499999999999996</v>
       </c>
       <c r="D61">
-        <v>13.261982</v>
+        <v>4.5999999999999996</v>
       </c>
       <c r="E61">
-        <v>47</v>
+        <v>12</v>
       </c>
       <c r="F61">
-        <v>6</v>
+        <v>2</v>
       </c>
       <c r="G61">
-        <v>2.2539999999999999E-3</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.2">
@@ -4124,22 +4270,22 @@
         <v>61</v>
       </c>
       <c r="B62">
-        <v>25.768913000000001</v>
+        <v>29.43</v>
       </c>
       <c r="C62">
-        <v>6.4284290000000004</v>
+        <v>9.5299999999999994</v>
       </c>
       <c r="D62">
-        <v>11.838996</v>
+        <v>7.06</v>
       </c>
       <c r="E62">
-        <v>47</v>
+        <v>11</v>
       </c>
       <c r="F62">
-        <v>7</v>
+        <v>2</v>
       </c>
       <c r="G62">
-        <v>2.0599999999999999E-4</v>
+        <v>0</v>
       </c>
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.2">
@@ -4147,22 +4293,22 @@
         <v>62</v>
       </c>
       <c r="B63">
-        <v>42.174145000000003</v>
+        <v>28.66</v>
       </c>
       <c r="C63">
-        <v>9.7995370000000008</v>
+        <v>11.04</v>
       </c>
       <c r="D63">
-        <v>17.116368999999999</v>
+        <v>9.14</v>
       </c>
       <c r="E63">
-        <v>46</v>
+        <v>13</v>
       </c>
       <c r="F63">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G63">
-        <v>3.2659999999999998E-3</v>
+        <v>0.01</v>
       </c>
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.2">
@@ -4170,22 +4316,22 @@
         <v>63</v>
       </c>
       <c r="B64">
-        <v>50.653114000000002</v>
+        <v>48.75</v>
       </c>
       <c r="C64">
-        <v>11.142860000000001</v>
+        <v>12.35</v>
       </c>
       <c r="D64">
-        <v>17.351396999999999</v>
+        <v>12.5</v>
       </c>
       <c r="E64">
-        <v>48</v>
+        <v>18</v>
       </c>
       <c r="F64">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G64">
-        <v>1.9203999999999999E-2</v>
+        <v>0.14000000000000001</v>
       </c>
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.2">
@@ -4193,22 +4339,22 @@
         <v>64</v>
       </c>
       <c r="B65">
-        <v>59.465423999999999</v>
+        <v>46.07</v>
       </c>
       <c r="C65">
-        <v>12.895859</v>
+        <v>12.13</v>
       </c>
       <c r="D65">
-        <v>15.098578</v>
+        <v>17.34</v>
       </c>
       <c r="E65">
-        <v>50</v>
+        <v>24</v>
       </c>
       <c r="F65">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="G65">
-        <v>0.179864</v>
+        <v>0.56000000000000005</v>
       </c>
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.2">
@@ -4216,22 +4362,22 @@
         <v>65</v>
       </c>
       <c r="B66">
-        <v>57.734195999999997</v>
+        <v>72.349999999999994</v>
       </c>
       <c r="C66">
-        <v>10.564776999999999</v>
+        <v>10.86</v>
       </c>
       <c r="D66">
-        <v>12.762147000000001</v>
+        <v>15.98</v>
       </c>
       <c r="E66">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="F66">
-        <v>7</v>
+        <v>1</v>
       </c>
       <c r="G66">
-        <v>0.38442500000000002</v>
+        <v>2.15</v>
       </c>
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.2">
@@ -4239,22 +4385,22 @@
         <v>66</v>
       </c>
       <c r="B67">
-        <v>77.249756000000005</v>
+        <v>76.260000000000005</v>
       </c>
       <c r="C67">
-        <v>7.641038</v>
+        <v>7.29</v>
       </c>
       <c r="D67">
-        <v>9.8777279999999994</v>
+        <v>11.36</v>
       </c>
       <c r="E67">
-        <v>49</v>
+        <v>37</v>
       </c>
       <c r="F67">
-        <v>8</v>
+        <v>1</v>
       </c>
       <c r="G67">
-        <v>1.3703419999999999</v>
+        <v>3.65</v>
       </c>
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.2">
@@ -4262,22 +4408,22 @@
         <v>67</v>
       </c>
       <c r="B68">
-        <v>75.877562999999995</v>
+        <v>65.38</v>
       </c>
       <c r="C68">
-        <v>4.0006300000000001</v>
+        <v>4.25</v>
       </c>
       <c r="D68">
-        <v>6.0574000000000003</v>
+        <v>3.69</v>
       </c>
       <c r="E68">
-        <v>45</v>
+        <v>38</v>
       </c>
       <c r="F68">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="G68">
-        <v>1.561923</v>
+        <v>5.58</v>
       </c>
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.2">
@@ -4285,22 +4431,22 @@
         <v>68</v>
       </c>
       <c r="B69">
-        <v>58.825797999999999</v>
+        <v>72.569999999999993</v>
       </c>
       <c r="C69">
-        <v>3.4767269999999999</v>
+        <v>2.41</v>
       </c>
       <c r="D69">
-        <v>2.3965200000000002</v>
+        <v>0</v>
       </c>
       <c r="E69">
-        <v>38</v>
+        <v>30</v>
       </c>
       <c r="F69">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G69">
-        <v>1.4598960000000001</v>
+        <v>1.39</v>
       </c>
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.2">
@@ -4308,10 +4454,10 @@
         <v>69</v>
       </c>
       <c r="B70">
-        <v>54.012954999999998</v>
+        <v>60.72</v>
       </c>
       <c r="C70">
-        <v>1.4737420000000001</v>
+        <v>0</v>
       </c>
       <c r="D70">
         <v>0</v>
@@ -4320,10 +4466,10 @@
         <v>29</v>
       </c>
       <c r="F70">
-        <v>5</v>
+        <v>1</v>
       </c>
       <c r="G70">
-        <v>0.65075499999999997</v>
+        <v>2.6</v>
       </c>
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.2">
@@ -4331,22 +4477,22 @@
         <v>70</v>
       </c>
       <c r="B71">
-        <v>44.467818999999999</v>
+        <v>43.18</v>
       </c>
       <c r="C71">
-        <v>0.15698300000000001</v>
+        <v>2.13</v>
       </c>
       <c r="D71">
-        <v>0.38599699999999998</v>
+        <v>0</v>
       </c>
       <c r="E71">
-        <v>24</v>
+        <v>28</v>
       </c>
       <c r="F71">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G71">
-        <v>0.114098</v>
+        <v>0.6</v>
       </c>
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.2">
@@ -4354,22 +4500,22 @@
         <v>71</v>
       </c>
       <c r="B72">
-        <v>28.922798</v>
+        <v>37.28</v>
       </c>
       <c r="C72">
-        <v>2.3013590000000002</v>
+        <v>2.96</v>
       </c>
       <c r="D72">
-        <v>0.368448</v>
+        <v>3.04</v>
       </c>
       <c r="E72">
-        <v>22</v>
+        <v>27</v>
       </c>
       <c r="F72">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G72">
-        <v>2.2356000000000001E-2</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.2">
@@ -4377,22 +4523,22 @@
         <v>72</v>
       </c>
       <c r="B73">
-        <v>29.444271000000001</v>
+        <v>22.39</v>
       </c>
       <c r="C73">
-        <v>5.6954260000000003</v>
+        <v>4.45</v>
       </c>
       <c r="D73">
-        <v>1.4273769999999999</v>
+        <v>2.99</v>
       </c>
       <c r="E73">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="F73">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="G73">
-        <v>3.2810000000000001E-3</v>
+        <v>0.01</v>
       </c>
     </row>
   </sheetData>

</xml_diff>